<commit_message>
Added attribute group import
</commit_message>
<xml_diff>
--- a/Resources/fixtures/minimal/init.xlsx
+++ b/Resources/fixtures/minimal/init.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="4" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="362" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="1" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="362" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="family main" sheetId="1" state="visible" r:id="rId2"/>
@@ -155,7 +155,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="227">
   <si>
     <t>en_US</t>
   </si>
@@ -380,9 +380,6 @@
   </si>
   <si>
     <t>Position</t>
-  </si>
-  <si>
-    <t>position</t>
   </si>
   <si>
     <t>Global</t>
@@ -976,7 +973,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
@@ -1043,10 +1040,6 @@
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="3" fontId="6" numFmtId="164" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="6" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="3" fontId="6" numFmtId="164" xfId="0">
@@ -1134,15 +1127,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>54000</xdr:colOff>
+      <xdr:colOff>81000</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>153720</xdr:rowOff>
+      <xdr:rowOff>145080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1034280</xdr:colOff>
+      <xdr:colOff>1060920</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>154080</xdr:rowOff>
+      <xdr:rowOff>145440</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1151,8 +1144,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="54000" y="316080"/>
-          <a:ext cx="6530040" cy="360"/>
+          <a:off x="81000" y="307440"/>
+          <a:ext cx="6529680" cy="360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1173,15 +1166,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>54000</xdr:colOff>
+      <xdr:colOff>81000</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>153720</xdr:rowOff>
+      <xdr:rowOff>145080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>406440</xdr:colOff>
+      <xdr:colOff>433440</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>154080</xdr:rowOff>
+      <xdr:rowOff>145440</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1190,7 +1183,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="54000" y="316080"/>
+          <a:off x="81000" y="307440"/>
           <a:ext cx="3480120" cy="360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1220,7 +1213,7 @@
   <dimension ref="A1:BC65536"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100">
-      <selection activeCell="A6" activeCellId="0" pane="topLeft" sqref="A6"/>
+      <selection activeCell="A6" activeCellId="1" pane="topLeft" sqref="3:3 A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1732,8 +1725,8 @@
   </sheetPr>
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100">
-      <selection activeCell="C19" activeCellId="0" pane="topLeft" sqref="C19"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100">
+      <selection activeCell="A3" activeCellId="0" pane="topLeft" sqref="3:3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1765,13 +1758,13 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="24.45" outlineLevel="0" r="3">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="17" t="s">
-        <v>75</v>
-      </c>
-      <c r="C3" s="0" t="s">
+      <c r="B3" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="16" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1783,7 +1776,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -1809,7 +1802,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100">
-      <selection activeCell="B18" activeCellId="0" pane="topLeft" sqref="B18"/>
+      <selection activeCell="B18" activeCellId="1" pane="topLeft" sqref="3:3 B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1822,7 +1815,7 @@
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.5" outlineLevel="0" r="1">
       <c r="A1" s="14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B1" s="14"/>
       <c r="C1" s="14"/>
@@ -1835,10 +1828,10 @@
         <v>5</v>
       </c>
       <c r="B2" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2" s="9" t="s">
         <v>78</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>79</v>
       </c>
       <c r="D2" s="16" t="s">
         <v>0</v>
@@ -1846,13 +1839,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="12.1" outlineLevel="0" r="3">
       <c r="A3" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>37</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D3" s="16" t="s">
         <v>38</v>
@@ -1881,7 +1874,7 @@
   <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100">
-      <selection activeCell="B13" activeCellId="0" pane="topLeft" sqref="B13"/>
+      <selection activeCell="B13" activeCellId="1" pane="topLeft" sqref="3:3 B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1896,66 +1889,66 @@
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="1">
       <c r="A1" s="14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B1" s="14"/>
       <c r="C1" s="14"/>
       <c r="D1" s="14"/>
       <c r="E1" s="14"/>
-      <c r="F1" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
+      <c r="F1" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="2">
       <c r="A2" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="B2" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="C2" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="D2" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="E2" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="F2" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="F2" s="15" t="s">
+      <c r="G2" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="G2" s="15" t="s">
+      <c r="H2" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="H2" s="15" t="s">
+      <c r="I2" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="I2" s="15" t="s">
+      <c r="J2" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="J2" s="15" t="s">
+      <c r="K2" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="K2" s="15" t="s">
+      <c r="L2" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="L2" s="15" t="s">
+      <c r="M2" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="M2" s="15" t="s">
+      <c r="N2" s="15" t="s">
         <v>96</v>
-      </c>
-      <c r="N2" s="15" t="s">
-        <v>97</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="23.6" outlineLevel="0" r="3">
@@ -1963,43 +1956,43 @@
         <v>37</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C3" s="9" t="s">
         <v>47</v>
       </c>
       <c r="D3" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="E3" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="F3" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="F3" s="15" t="s">
+      <c r="G3" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="G3" s="15" t="s">
+      <c r="H3" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="H3" s="15" t="s">
+      <c r="I3" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="I3" s="15" t="s">
+      <c r="J3" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="J3" s="15" t="s">
+      <c r="K3" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="K3" s="15" t="s">
+      <c r="L3" s="15" t="s">
         <v>106</v>
       </c>
-      <c r="L3" s="15" t="s">
+      <c r="M3" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="M3" s="15" t="s">
+      <c r="N3" s="15" t="s">
         <v>108</v>
-      </c>
-      <c r="N3" s="15" t="s">
-        <v>109</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="4">
@@ -2013,37 +2006,37 @@
         <v>0</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="19" t="s">
+      <c r="F4" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="G4" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="G4" s="19" t="s">
+      <c r="H4" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="H4" s="19" t="s">
+      <c r="I4" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="I4" s="19" t="s">
+      <c r="J4" s="18" t="s">
         <v>114</v>
       </c>
-      <c r="J4" s="19" t="s">
+      <c r="K4" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="K4" s="19" t="s">
+      <c r="L4" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="L4" s="19" t="s">
+      <c r="M4" s="18" t="s">
         <v>117</v>
       </c>
-      <c r="M4" s="19" t="s">
+      <c r="N4" s="18" t="s">
         <v>118</v>
-      </c>
-      <c r="N4" s="19" t="s">
-        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -2111,8 +2104,8 @@
   </sheetPr>
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100">
-      <selection activeCell="B16" activeCellId="0" pane="topLeft" sqref="B16"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100">
+      <selection activeCell="B16" activeCellId="1" pane="topLeft" sqref="3:3 B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2124,7 +2117,7 @@
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="1">
       <c r="A1" s="14" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B1" s="14"/>
       <c r="C1" s="15" t="s">
@@ -2133,10 +2126,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="2">
       <c r="A2" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="B2" s="9" t="s">
         <v>121</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>122</v>
       </c>
       <c r="C2" s="16" t="s">
         <v>0</v>
@@ -2147,7 +2140,7 @@
         <v>37</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C3" s="16" t="s">
         <v>38</v>
@@ -2157,8 +2150,8 @@
       <c r="A4" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="19" t="s">
-        <v>124</v>
+      <c r="C4" s="18" t="s">
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -2190,7 +2183,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100">
-      <selection activeCell="B30" activeCellId="0" pane="topLeft" sqref="B30"/>
+      <selection activeCell="B30" activeCellId="1" pane="topLeft" sqref="3:3 B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.1"/>
@@ -2202,10 +2195,10 @@
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="true" ht="23.85" outlineLevel="0" r="1" s="3">
       <c r="A1" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>125</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>126</v>
       </c>
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="2" s="3">
@@ -2213,12 +2206,12 @@
         <v>37</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="3">
       <c r="A3" s="0" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>69</v>
@@ -2226,90 +2219,90 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="4">
       <c r="A4" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="B4" s="0" t="s">
         <v>128</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>129</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="5">
       <c r="A5" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="B5" s="0" t="s">
         <v>130</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>131</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="6">
       <c r="A6" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="B6" s="0" t="s">
         <v>132</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>133</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="7">
       <c r="A7" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="B7" s="0" t="s">
         <v>134</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>135</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="8">
       <c r="A8" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="B8" s="0" t="s">
         <v>136</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>137</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="9">
       <c r="A9" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="B9" s="0" t="s">
         <v>138</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>139</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="10">
       <c r="A10" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="B10" s="0" t="s">
         <v>140</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>141</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="11">
       <c r="A11" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="B11" s="0" t="s">
         <v>142</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>143</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="12">
       <c r="A12" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="B12" s="0" t="s">
         <v>144</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>145</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="13">
       <c r="A13" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="B13" s="0" t="s">
         <v>146</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>147</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="14">
       <c r="A14" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="B14" s="0" t="s">
         <v>148</v>
-      </c>
-      <c r="B14" s="0" t="s">
-        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -2331,7 +2324,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100">
-      <selection activeCell="A3" activeCellId="0" pane="topLeft" sqref="A3"/>
+      <selection activeCell="A3" activeCellId="0" pane="topLeft" sqref="3:3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.1"/>
@@ -2343,10 +2336,10 @@
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="true" ht="23.85" outlineLevel="0" r="1" s="3">
       <c r="A1" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>125</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>126</v>
       </c>
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="2" s="3">
@@ -2354,79 +2347,79 @@
         <v>37</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="3">
       <c r="A3" s="0" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="4">
       <c r="A4" s="0" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="5">
       <c r="A5" s="0" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="6">
       <c r="A6" s="0" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="7">
       <c r="A7" s="0" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="8">
       <c r="A8" s="0" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="9">
       <c r="A9" s="0" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="10">
       <c r="A10" s="0" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="11">
       <c r="A11" s="0" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -2448,7 +2441,7 @@
   <dimension ref="1:89"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A73" view="normal" windowProtection="false" workbookViewId="0" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100">
-      <selection activeCell="A116" activeCellId="0" pane="topLeft" sqref="A116"/>
+      <selection activeCell="A116" activeCellId="1" pane="topLeft" sqref="3:3 A116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.1"/>
@@ -2460,7 +2453,7 @@
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="true" ht="12.65" outlineLevel="0" r="1" s="3">
       <c r="A1" s="9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B1" s="9"/>
       <c r="AMJ1" s="0"/>
@@ -2470,704 +2463,704 @@
         <v>39</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="AMJ2" s="0"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="3">
       <c r="A3" s="0" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="4">
       <c r="A4" s="0" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="5">
       <c r="A5" s="0" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="6">
       <c r="A6" s="0" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="7">
       <c r="A7" s="0" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="8">
       <c r="A8" s="0" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="9">
       <c r="A9" s="0" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="10">
       <c r="A10" s="0" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="11">
       <c r="A11" s="0" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="12">
       <c r="A12" s="0" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="13">
       <c r="A13" s="0" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="14">
       <c r="A14" s="0" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="15">
       <c r="A15" s="0" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="16">
       <c r="A16" s="0" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="17">
       <c r="A17" s="0" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="18">
       <c r="A18" s="0" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="19">
       <c r="A19" s="0" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="20">
       <c r="A20" s="0" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="21">
       <c r="A21" s="0" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="22">
       <c r="A22" s="0" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="23">
       <c r="A23" s="0" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="24">
       <c r="A24" s="0" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="25">
       <c r="A25" s="0" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="26">
       <c r="A26" s="0" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="27">
       <c r="A27" s="0" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="28">
       <c r="A28" s="0" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="29">
       <c r="A29" s="0" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="30">
       <c r="A30" s="0" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="31">
       <c r="A31" s="0" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="32">
       <c r="A32" s="0" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="33">
       <c r="A33" s="0" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="34">
       <c r="A34" s="0" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="35">
       <c r="A35" s="0" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="36">
       <c r="A36" s="0" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="37">
       <c r="A37" s="0" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="38">
       <c r="A38" s="0" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="39">
       <c r="A39" s="0" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="40">
       <c r="A40" s="0" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="41">
       <c r="A41" s="0" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="42">
       <c r="A42" s="0" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="43">
       <c r="A43" s="0" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="44">
       <c r="A44" s="0" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="45">
       <c r="A45" s="0" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="46">
       <c r="A46" s="0" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="47">
       <c r="A47" s="0" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="48">
       <c r="A48" s="0" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="49">
       <c r="A49" s="0" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="50">
       <c r="A50" s="0" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="51">
       <c r="A51" s="0" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="52">
       <c r="A52" s="0" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="53">
       <c r="A53" s="0" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="54">
       <c r="A54" s="0" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="55">
       <c r="A55" s="0" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="56">
       <c r="A56" s="0" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="57">
       <c r="A57" s="0" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="58">
       <c r="A58" s="0" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="59">
       <c r="A59" s="0" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="60">
       <c r="A60" s="0" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="61">
       <c r="A61" s="0" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="62">
       <c r="A62" s="0" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="63">
       <c r="A63" s="0" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="64">
       <c r="A64" s="0" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="65">
       <c r="A65" s="0" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="66">
       <c r="A66" s="0" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="67">
       <c r="A67" s="0" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="68">
       <c r="A68" s="0" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="69">
       <c r="A69" s="0" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="70">
       <c r="A70" s="0" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="71">
       <c r="A71" s="0" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="72">
       <c r="A72" s="0" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="73">
       <c r="A73" s="0" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="74">
       <c r="A74" s="0" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="75">
       <c r="A75" s="0" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="76">
       <c r="A76" s="0" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="77">
       <c r="A77" s="0" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="78">
       <c r="A78" s="0" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="79">
       <c r="A79" s="0" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="80">
       <c r="A80" s="0" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="81">
       <c r="A81" s="0" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="82">
       <c r="A82" s="0" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="83">
       <c r="A83" s="0" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="84">
       <c r="A84" s="0" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="85">
       <c r="A85" s="0" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="86">
       <c r="A86" s="0" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="87">
       <c r="A87" s="0" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="88">
       <c r="A88" s="0" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="89">
       <c r="A89" s="0" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added category and channels import
</commit_message>
<xml_diff>
--- a/Resources/fixtures/minimal/init.xlsx
+++ b/Resources/fixtures/minimal/init.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="1" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="362" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="362" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="family main" sheetId="1" state="visible" r:id="rId2"/>
@@ -1210,13 +1210,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:BC65536"/>
+  <dimension ref="A1:BC7"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100">
-      <selection activeCell="A6" activeCellId="1" pane="topLeft" sqref="3:3 A6"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="B1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100">
+      <selection activeCell="F7" activeCellId="0" pane="topLeft" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.7755102040816"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.7755102040816"/>
@@ -1289,6 +1289,7 @@
       <c r="BB2" s="0"/>
       <c r="BC2" s="0"/>
     </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="3"/>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="4">
       <c r="A4" s="4" t="s">
         <v>5</v>
@@ -1612,8 +1613,6 @@
         <v>1</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="1048575"/>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="1048576"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="C4:AE4"/>
@@ -1725,8 +1724,8 @@
   </sheetPr>
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100">
-      <selection activeCell="A3" activeCellId="0" pane="topLeft" sqref="3:3"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100">
+      <selection activeCell="A3" activeCellId="0" pane="topLeft" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1802,7 +1801,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100">
-      <selection activeCell="B18" activeCellId="1" pane="topLeft" sqref="3:3 B18"/>
+      <selection activeCell="B18" activeCellId="0" pane="topLeft" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1874,7 +1873,7 @@
   <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100">
-      <selection activeCell="B13" activeCellId="1" pane="topLeft" sqref="3:3 B13"/>
+      <selection activeCell="B13" activeCellId="0" pane="topLeft" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2105,7 +2104,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100">
-      <selection activeCell="B16" activeCellId="1" pane="topLeft" sqref="3:3 B16"/>
+      <selection activeCell="B16" activeCellId="0" pane="topLeft" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2183,7 +2182,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100">
-      <selection activeCell="B30" activeCellId="1" pane="topLeft" sqref="3:3 B30"/>
+      <selection activeCell="B30" activeCellId="0" pane="topLeft" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.1"/>
@@ -2324,7 +2323,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100">
-      <selection activeCell="A3" activeCellId="0" pane="topLeft" sqref="3:3"/>
+      <selection activeCell="A3" activeCellId="0" pane="topLeft" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.1"/>
@@ -2441,7 +2440,7 @@
   <dimension ref="1:89"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A73" view="normal" windowProtection="false" workbookViewId="0" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100">
-      <selection activeCell="A116" activeCellId="1" pane="topLeft" sqref="3:3 A116"/>
+      <selection activeCell="A116" activeCellId="0" pane="topLeft" sqref="A116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.1"/>

</xml_diff>

<commit_message>
Added doc in the xlsx files
</commit_message>
<xml_diff>
--- a/Resources/fixtures/minimal/init.xlsx
+++ b/Resources/fixtures/minimal/init.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="6990" tabRatio="226" firstSheet="4" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="6990" tabRatio="226" firstSheet="5" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="10" r:id="rId1"/>
@@ -59,7 +59,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">Insert the name of the locales, seperatated by ",".
+          <t xml:space="preserve">Insert the name of the locales, separated by ",".
 For example : "en_US, fr_FR"
 </t>
         </r>
@@ -77,6 +77,20 @@
           <t>Insert the allowed extensions, separated by a comma.
 For example : 
 jpg, jpeg, png</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AD5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Determines how many characters should be typed for select attributes before an option is presented.
+This should be used for attributes which have a large number of options.</t>
         </r>
       </text>
     </comment>
@@ -894,9 +908,6 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">If an attribute is present in multiple families, only fill the blue columns (attribute properties) once </t>
-  </si>
-  <si>
     <t>Attribute groups</t>
   </si>
   <si>
@@ -1065,6 +1076,9 @@
   </si>
   <si>
     <t>The codes for label translations are always of the form "label-&lt;locale&gt;". For example, the french label has the code "label-fr_FR"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If an attribute is present in multiple families, only fill the blue and pink columns (attribute properties and translations) once </t>
   </si>
 </sst>
 </file>
@@ -1187,7 +1201,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1228,15 +1242,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1269,6 +1274,18 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1913,8 +1930,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1923,32 +1940,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="22" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="21" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B5" s="26" t="s">
+      <c r="B5" s="23" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="24" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B7" s="27" t="s">
-        <v>245</v>
+      <c r="B7" s="24" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="24" t="s">
+      <c r="B9" s="21" t="s">
         <v>232</v>
       </c>
     </row>
@@ -1964,102 +1981,102 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>235</v>
+        <v>276</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="24" t="s">
-        <v>236</v>
+      <c r="B16" s="21" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B20" s="21" t="s">
         <v>237</v>
-      </c>
-    </row>
-    <row r="20" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B20" s="24" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B25" s="21" t="s">
         <v>240</v>
-      </c>
-    </row>
-    <row r="25" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B25" s="24" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B28" s="27" t="s">
-        <v>244</v>
+      <c r="B28" s="24" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="30" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B30" s="24" t="s">
-        <v>246</v>
+      <c r="B30" s="21" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="32" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B35" s="24" t="s">
-        <v>270</v>
+      <c r="B35" s="21" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B39" s="21" t="s">
         <v>271</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B39" s="24" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+      <c r="A44" s="29" t="s">
         <v>273</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" ht="18" x14ac:dyDescent="0.25">
-      <c r="A44" s="32" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
   </sheetData>
@@ -3058,8 +3075,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BB8"/>
   <sheetViews>
-    <sheetView topLeftCell="V1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="AE18" sqref="AE18"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3068,15 +3085,15 @@
     <col min="2" max="3" width="24.7109375"/>
     <col min="4" max="4" width="23.7109375"/>
     <col min="5" max="5" width="16.7109375"/>
-    <col min="6" max="6" width="19.7109375" style="19"/>
-    <col min="7" max="7" width="14" style="19"/>
-    <col min="8" max="8" width="13" style="19"/>
-    <col min="9" max="9" width="25.85546875" style="19"/>
-    <col min="10" max="10" width="25.140625" style="19"/>
+    <col min="6" max="6" width="19.7109375" style="16"/>
+    <col min="7" max="7" width="14" style="16"/>
+    <col min="8" max="8" width="13" style="16"/>
+    <col min="9" max="9" width="25.85546875" style="16"/>
+    <col min="10" max="10" width="25.140625" style="16"/>
     <col min="11" max="11" width="20"/>
-    <col min="12" max="12" width="23.5703125" style="19"/>
-    <col min="13" max="13" width="23.85546875" style="19"/>
-    <col min="14" max="14" width="20.7109375" style="19"/>
+    <col min="12" max="12" width="23.5703125" style="16"/>
+    <col min="13" max="13" width="23.85546875" style="16"/>
+    <col min="14" max="14" width="20.7109375" style="16"/>
     <col min="15" max="15" width="20.42578125"/>
     <col min="16" max="16" width="19.28515625"/>
     <col min="17" max="18" width="17.28515625"/>
@@ -3090,7 +3107,7 @@
     <col min="28" max="28" width="21"/>
     <col min="29" max="29" width="22"/>
     <col min="30" max="30" width="23.42578125"/>
-    <col min="31" max="31" width="14.85546875" style="19"/>
+    <col min="31" max="31" width="14.85546875" style="16"/>
     <col min="32" max="40" width="13.42578125"/>
     <col min="41" max="41" width="16.85546875"/>
     <col min="42" max="42" width="19.140625"/>
@@ -3133,137 +3150,137 @@
       <c r="BA2"/>
       <c r="BB2"/>
     </row>
-    <row r="4" spans="1:54" s="22" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="28"/>
-      <c r="B4" s="28"/>
+    <row r="4" spans="1:54" s="19" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="25"/>
+      <c r="B4" s="25"/>
       <c r="C4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="D4" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
-      <c r="J4" s="16"/>
-      <c r="K4" s="16"/>
-      <c r="L4" s="16"/>
-      <c r="M4" s="16"/>
-      <c r="N4" s="16"/>
-      <c r="O4" s="16"/>
-      <c r="P4" s="16"/>
-      <c r="Q4" s="16"/>
-      <c r="R4" s="16"/>
-      <c r="S4" s="16"/>
-      <c r="T4" s="16"/>
-      <c r="U4" s="16"/>
-      <c r="V4" s="16"/>
-      <c r="W4" s="16"/>
-      <c r="X4" s="16"/>
-      <c r="Y4" s="16"/>
-      <c r="Z4" s="16"/>
-      <c r="AA4" s="16"/>
-      <c r="AB4" s="16"/>
-      <c r="AC4" s="16"/>
-      <c r="AD4" s="16"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="30"/>
+      <c r="J4" s="30"/>
+      <c r="K4" s="30"/>
+      <c r="L4" s="30"/>
+      <c r="M4" s="30"/>
+      <c r="N4" s="30"/>
+      <c r="O4" s="30"/>
+      <c r="P4" s="30"/>
+      <c r="Q4" s="30"/>
+      <c r="R4" s="30"/>
+      <c r="S4" s="30"/>
+      <c r="T4" s="30"/>
+      <c r="U4" s="30"/>
+      <c r="V4" s="30"/>
+      <c r="W4" s="30"/>
+      <c r="X4" s="30"/>
+      <c r="Y4" s="30"/>
+      <c r="Z4" s="30"/>
+      <c r="AA4" s="30"/>
+      <c r="AB4" s="30"/>
+      <c r="AC4" s="30"/>
+      <c r="AD4" s="30"/>
       <c r="AE4" s="7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="22" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="28" t="s">
+    <row r="5" spans="1:54" s="19" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="28" t="s">
+      <c r="B5" s="25" t="s">
         <v>9</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="29" t="s">
+      <c r="D5" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="29" t="s">
+      <c r="E5" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="29" t="s">
+      <c r="F5" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="29" t="s">
+      <c r="G5" s="26" t="s">
+        <v>248</v>
+      </c>
+      <c r="H5" s="26" t="s">
         <v>249</v>
       </c>
-      <c r="H5" s="29" t="s">
+      <c r="I5" s="26" t="s">
         <v>250</v>
       </c>
-      <c r="I5" s="29" t="s">
+      <c r="J5" s="26" t="s">
         <v>251</v>
       </c>
-      <c r="J5" s="29" t="s">
+      <c r="K5" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="L5" s="26" t="s">
         <v>252</v>
       </c>
-      <c r="K5" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="L5" s="29" t="s">
+      <c r="M5" s="26" t="s">
         <v>253</v>
       </c>
-      <c r="M5" s="29" t="s">
+      <c r="N5" s="26" t="s">
         <v>254</v>
       </c>
-      <c r="N5" s="29" t="s">
-        <v>255</v>
-      </c>
-      <c r="O5" s="29" t="s">
+      <c r="O5" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="P5" s="29" t="s">
+      <c r="P5" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="Q5" s="29" t="s">
+      <c r="Q5" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="R5" s="29" t="s">
+      <c r="R5" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="S5" s="29" t="s">
+      <c r="S5" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="T5" s="29" t="s">
+      <c r="T5" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="U5" s="29" t="s">
+      <c r="U5" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="V5" s="29" t="s">
+      <c r="V5" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="W5" s="29" t="s">
+      <c r="W5" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="X5" s="29" t="s">
+      <c r="X5" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="Y5" s="29" t="s">
+      <c r="Y5" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="Z5" s="29" t="s">
+      <c r="Z5" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="AA5" s="29" t="s">
+      <c r="AA5" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="AB5" s="29" t="s">
+      <c r="AB5" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="AC5" s="29" t="s">
+      <c r="AC5" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="AD5" s="29" t="s">
+      <c r="AD5" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="AE5" s="7" t="s">
+      <c r="AE5" s="33" t="s">
         <v>2</v>
       </c>
     </row>
@@ -3283,31 +3300,31 @@
       <c r="E6" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="F6" s="20" t="s">
+      <c r="F6" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="G6" s="20" t="s">
+      <c r="G6" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="H6" s="20" t="s">
+      <c r="H6" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="I6" s="20" t="s">
+      <c r="I6" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="J6" s="20" t="s">
+      <c r="J6" s="17" t="s">
         <v>39</v>
       </c>
       <c r="K6" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="L6" s="20" t="s">
+      <c r="L6" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="M6" s="20" t="s">
+      <c r="M6" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="N6" s="20" t="s">
+      <c r="N6" s="17" t="s">
         <v>43</v>
       </c>
       <c r="O6" s="9" t="s">
@@ -3358,7 +3375,7 @@
       <c r="AD6" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="AE6" s="23"/>
+      <c r="AE6" s="20"/>
       <c r="AY6"/>
       <c r="AZ6"/>
       <c r="BA6"/>
@@ -3377,29 +3394,29 @@
       <c r="E7" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="F7" s="19">
+      <c r="F7" s="16">
         <v>1</v>
       </c>
-      <c r="G7" s="21">
+      <c r="G7" s="18">
         <v>0</v>
       </c>
-      <c r="H7" s="21">
+      <c r="H7" s="18">
         <v>1</v>
       </c>
-      <c r="I7" s="21">
+      <c r="I7" s="18">
         <v>1</v>
       </c>
-      <c r="J7" s="21">
+      <c r="J7" s="18">
         <v>0</v>
       </c>
       <c r="K7" s="11"/>
-      <c r="L7" s="21">
+      <c r="L7" s="18">
         <v>0</v>
       </c>
-      <c r="M7" s="21">
+      <c r="M7" s="18">
         <v>1</v>
       </c>
-      <c r="N7" s="21">
+      <c r="N7" s="18">
         <v>1</v>
       </c>
       <c r="O7" s="11"/>
@@ -3417,7 +3434,7 @@
       <c r="AB7" s="11"/>
       <c r="AC7" s="11"/>
       <c r="AD7" s="11"/>
-      <c r="AE7" s="21">
+      <c r="AE7" s="18">
         <v>1</v>
       </c>
       <c r="AF7" s="11"/>
@@ -3462,31 +3479,31 @@
       <c r="E8" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="F8" s="19">
+      <c r="F8" s="16">
         <v>2</v>
       </c>
-      <c r="G8" s="19">
+      <c r="G8" s="16">
         <v>0</v>
       </c>
-      <c r="H8" s="19">
+      <c r="H8" s="16">
         <v>0</v>
       </c>
-      <c r="I8" s="19">
+      <c r="I8" s="16">
         <v>1</v>
       </c>
-      <c r="J8" s="19">
+      <c r="J8" s="16">
         <v>0</v>
       </c>
-      <c r="L8" s="19">
+      <c r="L8" s="16">
         <v>0</v>
       </c>
-      <c r="M8" s="19">
+      <c r="M8" s="16">
         <v>1</v>
       </c>
-      <c r="N8" s="19">
+      <c r="N8" s="16">
         <v>1</v>
       </c>
-      <c r="AE8" s="19">
+      <c r="AE8" s="16">
         <v>1</v>
       </c>
     </row>
@@ -3494,7 +3511,7 @@
   <mergeCells count="1">
     <mergeCell ref="D4:AD4"/>
   </mergeCells>
-  <dataValidations count="19">
+  <dataValidations count="17">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AO7:AP7 AU7:AW7">
       <formula1>ouinon</formula1>
       <formula2>0</formula2>
@@ -3531,19 +3548,11 @@
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V7">
-      <formula1>"0,1"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q7">
       <formula1>ouinon</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U7">
-      <formula1>"0,1"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G7:J1048576 L7:N1048576 R7:R1048576 B7:B1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G7:J1048576 L7:N1048576 R7:R1048576 B7:B1048576 U7:V1048576">
       <formula1>boolean_choices</formula1>
     </dataValidation>
     <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O7:O1048576">
@@ -3619,10 +3628,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="17"/>
+      <c r="B1" s="31"/>
       <c r="C1" s="13" t="s">
         <v>5</v>
       </c>
@@ -3686,11 +3695,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
       <c r="D1" s="13" t="s">
         <v>5</v>
       </c>
@@ -3743,7 +3752,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -3758,24 +3767,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="31" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="18" t="s">
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="32" t="s">
         <v>78</v>
       </c>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32"/>
+      <c r="L1" s="32"/>
+      <c r="M1" s="32"/>
+      <c r="N1" s="32"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
@@ -4003,10 +4012,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="31" t="s">
         <v>115</v>
       </c>
-      <c r="B1" s="17"/>
+      <c r="B1" s="31"/>
       <c r="C1" s="13" t="s">
         <v>5</v>
       </c>
@@ -4072,17 +4081,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="17" t="s">
-        <v>256</v>
-      </c>
-      <c r="B1" s="17"/>
+      <c r="A1" s="31" t="s">
+        <v>255</v>
+      </c>
+      <c r="B1" s="31"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
         <v>30</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="3" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
@@ -4090,12 +4099,12 @@
         <v>30</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -4103,7 +4112,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -4128,32 +4137,32 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="25.7109375" style="12" customWidth="1"/>
-    <col min="2" max="2" width="50.140625" style="31" customWidth="1"/>
+    <col min="2" max="2" width="50.140625" style="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="31" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" s="28" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="31" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="29" t="s">
-        <v>269</v>
+    <row r="2" spans="1:2" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="26" t="s">
+        <v>268</v>
       </c>
       <c r="B2" s="13" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" s="31" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" s="28" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>30</v>
       </c>
@@ -4163,34 +4172,34 @@
     </row>
     <row r="4" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
+        <v>259</v>
+      </c>
+      <c r="B4" s="27" t="s">
         <v>260</v>
-      </c>
-      <c r="B4" s="30" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
+        <v>261</v>
+      </c>
+      <c r="B5" s="28" t="s">
         <v>262</v>
-      </c>
-      <c r="B5" s="31" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
+        <v>263</v>
+      </c>
+      <c r="B6" s="28" t="s">
         <v>264</v>
-      </c>
-      <c r="B6" s="31" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
+        <v>265</v>
+      </c>
+      <c r="B7" s="28" t="s">
         <v>266</v>
-      </c>
-      <c r="B7" s="31" t="s">
-        <v>267</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Corrected validation bug on Excel 2007
</commit_message>
<xml_diff>
--- a/Resources/fixtures/minimal/init.xlsx
+++ b/Resources/fixtures/minimal/init.xlsx
@@ -4,27 +4,33 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="6990" tabRatio="226" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="6990" tabRatio="226" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="10" r:id="rId1"/>
-    <sheet name="family main" sheetId="1" r:id="rId2"/>
-    <sheet name="attribute_groups" sheetId="2" r:id="rId3"/>
-    <sheet name="options" sheetId="3" r:id="rId4"/>
-    <sheet name="channels" sheetId="4" r:id="rId5"/>
-    <sheet name="categories" sheetId="5" r:id="rId6"/>
-    <sheet name="group_types" sheetId="11" r:id="rId7"/>
-    <sheet name="association_types" sheetId="14" r:id="rId8"/>
-    <sheet name="choices" sheetId="9" state="hidden" r:id="rId9"/>
-    <sheet name="attribute_types" sheetId="6" state="hidden" r:id="rId10"/>
-    <sheet name="metric_types" sheetId="7" state="hidden" r:id="rId11"/>
-    <sheet name="metric_units" sheetId="8" state="hidden" r:id="rId12"/>
+    <sheet name="attributes" sheetId="15" r:id="rId2"/>
+    <sheet name="family main" sheetId="1" r:id="rId3"/>
+    <sheet name="attribute_groups" sheetId="2" r:id="rId4"/>
+    <sheet name="options" sheetId="3" r:id="rId5"/>
+    <sheet name="channels" sheetId="4" r:id="rId6"/>
+    <sheet name="categories" sheetId="5" r:id="rId7"/>
+    <sheet name="group_types" sheetId="11" r:id="rId8"/>
+    <sheet name="association_types" sheetId="14" r:id="rId9"/>
+    <sheet name="choices" sheetId="9" state="hidden" r:id="rId10"/>
+    <sheet name="attribute_types" sheetId="6" state="hidden" r:id="rId11"/>
+    <sheet name="metric_types" sheetId="7" state="hidden" r:id="rId12"/>
+    <sheet name="metric_units" sheetId="8" state="hidden" r:id="rId13"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2">attribute_groups!$A$4:$C$4</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1">'family main'!$C$6:$BA$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3">attribute_groups!$A$4:$C$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1">attributes!$B$6:$AZ$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2">'family main'!$C$6:$BB$9</definedName>
+    <definedName name="attribute_groups">attribute_groups!$A$4:$A$100</definedName>
+    <definedName name="attribute_types">attribute_types!$B$3:$B$14</definedName>
     <definedName name="boolean_choices">choices!$A$1:$A$2</definedName>
     <definedName name="date_choices">choices!$C$1:$C$3</definedName>
+    <definedName name="metric_types">metric_types!$B$3:$B$11</definedName>
+    <definedName name="metric_units">metric_units!$B$3:$B$89</definedName>
     <definedName name="validation_choices">choices!$B$1:$B$3</definedName>
   </definedNames>
   <calcPr calcId="0" iterateDelta="1E-4"/>
@@ -37,20 +43,7 @@
     <author>SMILE</author>
   </authors>
   <commentList>
-    <comment ref="AE4" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Set to 1 if the attribute is required in this family for the concerned channel.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="K5" authorId="0">
+    <comment ref="J5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -104,6 +97,73 @@
     <author>SMILE</author>
   </authors>
   <commentList>
+    <comment ref="AF4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Set to 1 if the attribute is required in this family for the concerned channel.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Insert the name of the locales, separated by ",".
+For example : "en_US, fr_FR"
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AD5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Insert the allowed extensions, separated by a comma.
+For example : 
+jpg, jpeg, png</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AE5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Determines how many characters should be typed for select attributes before an option is presented.
+This should be used for attributes which have a large number of options.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>SMILE</author>
+  </authors>
+  <commentList>
     <comment ref="C2" authorId="0">
       <text>
         <r>
@@ -121,7 +181,7 @@
 </comments>
 </file>
 
-<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>SMILE</author>
@@ -160,7 +220,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="274">
   <si>
     <t>en_US</t>
   </si>
@@ -1063,6 +1123,36 @@
       </rPr>
       <t>save this file with another extension than xlsx</t>
     </r>
+  </si>
+  <si>
+    <t>Default value</t>
+  </si>
+  <si>
+    <t>default_value</t>
+  </si>
+  <si>
+    <t>Attributes tab</t>
+  </si>
+  <si>
+    <t>The attributes tab can be used to define the properties of attributes which are not linked to families, or which are shared by families.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">This tab can be duplicated to shorten the list. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>All attributes tab titles should start with "attributes"</t>
+    </r>
+  </si>
+  <si>
+    <t>Common and unaffected attribute properties</t>
   </si>
 </sst>
 </file>
@@ -1909,10 +1999,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B48"/>
+  <dimension ref="A1:B53"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1950,118 +2040,139 @@
         <v>234</v>
       </c>
     </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B9" s="24"/>
+    </row>
     <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="21" t="s">
-        <v>222</v>
-      </c>
+        <v>270</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B11" s="24"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B12" t="s">
-        <v>223</v>
+      <c r="B12" s="23" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B15" s="21" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
         <v>224</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B14" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B15" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B17" s="21" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="21" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B21" s="21" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B23" t="s">
-        <v>228</v>
+        <v>266</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B22" s="21" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="26" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B26" s="21" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="29" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B29" s="24" t="s">
-        <v>233</v>
+      <c r="B29" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="31" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B31" s="21" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B34" s="24" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B36" s="21" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B33" t="s">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B38" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B34" t="s">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B39" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B36" s="21" t="s">
+    <row r="41" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B41" s="21" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B38" t="s">
+    <row r="43" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B43" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="21" t="s">
+    <row r="45" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B45" s="21" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B42" t="s">
+    <row r="47" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B47" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="18" x14ac:dyDescent="0.25">
-      <c r="A45" s="29" t="s">
+    <row r="50" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+      <c r="A50" s="29" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B47" t="s">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B52" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B48" t="s">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B53" t="s">
         <v>265</v>
       </c>
     </row>
@@ -2073,10 +2184,55 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C1" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>213</v>
+      </c>
+      <c r="C2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>214</v>
+      </c>
+      <c r="C3" t="s">
+        <v>217</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2208,12 +2364,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2321,12 +2477,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMJ89"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="B3" sqref="B3:B89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3060,92 +3216,77 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BB8"/>
+  <dimension ref="A1:BA8"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView topLeftCell="V1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="AA15" sqref="AA15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.7109375"/>
-    <col min="2" max="3" width="24.7109375"/>
-    <col min="4" max="4" width="23.7109375"/>
-    <col min="5" max="5" width="16.7109375"/>
-    <col min="6" max="6" width="19.7109375" style="16"/>
-    <col min="7" max="7" width="14" style="16"/>
-    <col min="8" max="8" width="13" style="16"/>
-    <col min="9" max="9" width="25.85546875" style="16"/>
-    <col min="10" max="10" width="25.140625" style="16"/>
-    <col min="11" max="11" width="20"/>
-    <col min="12" max="12" width="23.5703125" style="16"/>
-    <col min="13" max="13" width="23.85546875" style="16"/>
-    <col min="14" max="14" width="20.7109375" style="16"/>
-    <col min="15" max="15" width="20.42578125"/>
-    <col min="16" max="16" width="19.28515625"/>
-    <col min="17" max="18" width="17.28515625"/>
-    <col min="19" max="19" width="16.5703125"/>
-    <col min="20" max="20" width="19"/>
-    <col min="21" max="22" width="18.7109375"/>
-    <col min="23" max="24" width="13.42578125"/>
-    <col min="25" max="25" width="19.85546875"/>
-    <col min="26" max="26" width="13.42578125"/>
-    <col min="27" max="27" width="18.140625"/>
-    <col min="28" max="28" width="21"/>
-    <col min="29" max="29" width="22"/>
-    <col min="30" max="30" width="23.42578125"/>
-    <col min="31" max="31" width="14.85546875" style="16"/>
-    <col min="32" max="40" width="13.42578125"/>
-    <col min="41" max="41" width="16.85546875"/>
-    <col min="42" max="42" width="19.140625"/>
-    <col min="43" max="43" width="16.28515625"/>
-    <col min="44" max="46" width="13.42578125"/>
-    <col min="47" max="47" width="19.140625"/>
-    <col min="48" max="50" width="18.140625"/>
-    <col min="51" max="51" width="0" style="2" hidden="1"/>
-    <col min="52" max="52" width="0" style="3" hidden="1"/>
-    <col min="53" max="53" width="0" style="2" hidden="1"/>
-    <col min="54" max="54" width="17.140625" style="2"/>
-    <col min="55" max="1025" width="17.140625"/>
+    <col min="1" max="1" width="25" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" style="16" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" style="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" style="16" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.85546875" style="16" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" style="16" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" style="16" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23.42578125" style="16" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.5703125" style="16" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.28515625" style="16" customWidth="1"/>
+    <col min="15" max="15" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="17" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="14" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="19" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="21" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="9.140625" style="2"/>
+    <col min="51" max="51" width="9.140625" style="3"/>
+    <col min="52" max="53" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:53" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="24" t="s">
+        <v>273</v>
+      </c>
+      <c r="C1" s="4"/>
       <c r="D1" s="4"/>
-      <c r="E1" s="4" t="s">
-        <v>0</v>
-      </c>
+      <c r="AX1"/>
       <c r="AY1"/>
       <c r="AZ1"/>
       <c r="BA1"/>
-      <c r="BB1"/>
-    </row>
-    <row r="2" spans="1:54" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>4</v>
-      </c>
+    </row>
+    <row r="2" spans="1:53" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="AX2"/>
       <c r="AY2"/>
       <c r="AZ2"/>
       <c r="BA2"/>
-      <c r="BB2"/>
-    </row>
-    <row r="4" spans="1:54" s="19" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:53" s="19" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="25"/>
-      <c r="B4" s="25"/>
-      <c r="C4" s="6" t="s">
+      <c r="B4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="31" t="s">
+      <c r="C4" s="31" t="s">
         <v>6</v>
       </c>
+      <c r="D4" s="31"/>
       <c r="E4" s="31"/>
       <c r="F4" s="31"/>
       <c r="G4" s="31"/>
@@ -3172,52 +3313,49 @@
       <c r="AB4" s="31"/>
       <c r="AC4" s="31"/>
       <c r="AD4" s="31"/>
-      <c r="AE4" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:54" s="19" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:53" s="19" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="6" t="s">
+      <c r="B5" s="6" t="s">
         <v>0</v>
       </c>
+      <c r="C5" s="26" t="s">
+        <v>10</v>
+      </c>
       <c r="D5" s="26" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E5" s="26" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F5" s="26" t="s">
-        <v>12</v>
+        <v>238</v>
       </c>
       <c r="G5" s="26" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="H5" s="26" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="I5" s="26" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="J5" s="26" t="s">
-        <v>241</v>
+        <v>13</v>
       </c>
       <c r="K5" s="26" t="s">
-        <v>13</v>
+        <v>242</v>
       </c>
       <c r="L5" s="26" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="M5" s="26" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="N5" s="26" t="s">
-        <v>244</v>
+        <v>268</v>
       </c>
       <c r="O5" s="26" t="s">
         <v>14</v>
@@ -3267,52 +3405,49 @@
       <c r="AD5" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="AE5" s="30" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:54" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:53" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6" s="8" t="s">
+      <c r="B6" s="8" t="s">
         <v>32</v>
       </c>
+      <c r="C6" s="9" t="s">
+        <v>33</v>
+      </c>
       <c r="D6" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="E6" s="9" t="s">
         <v>34</v>
       </c>
+      <c r="E6" s="17" t="s">
+        <v>35</v>
+      </c>
       <c r="F6" s="17" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G6" s="17" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H6" s="17" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I6" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="J6" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="K6" s="9" t="s">
+      <c r="J6" s="9" t="s">
         <v>40</v>
       </c>
+      <c r="K6" s="17" t="s">
+        <v>41</v>
+      </c>
       <c r="L6" s="17" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="M6" s="17" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="N6" s="17" t="s">
-        <v>43</v>
+        <v>269</v>
       </c>
       <c r="O6" s="9" t="s">
         <v>44</v>
@@ -3362,50 +3497,50 @@
       <c r="AD6" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="AE6" s="20"/>
+      <c r="AX6"/>
       <c r="AY6"/>
       <c r="AZ6"/>
       <c r="BA6"/>
-      <c r="BB6"/>
-    </row>
-    <row r="7" spans="1:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="C7" t="s">
+      <c r="B7" t="s">
         <v>61</v>
       </c>
+      <c r="C7" s="10" t="s">
+        <v>62</v>
+      </c>
       <c r="D7" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="E7" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="F7" s="16">
+      <c r="E7" s="16">
         <v>1</v>
       </c>
+      <c r="F7" s="18">
+        <v>0</v>
+      </c>
       <c r="G7" s="18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7" s="18">
         <v>1</v>
       </c>
       <c r="I7" s="18">
+        <v>0</v>
+      </c>
+      <c r="J7" s="11"/>
+      <c r="K7" s="18">
+        <v>0</v>
+      </c>
+      <c r="L7" s="18">
         <v>1</v>
-      </c>
-      <c r="J7" s="18">
-        <v>0</v>
-      </c>
-      <c r="K7" s="11"/>
-      <c r="L7" s="18">
-        <v>0</v>
       </c>
       <c r="M7" s="18">
         <v>1</v>
       </c>
-      <c r="N7" s="18">
-        <v>1</v>
-      </c>
+      <c r="N7" s="18"/>
       <c r="O7" s="11"/>
       <c r="Q7" s="11"/>
       <c r="R7" s="11"/>
@@ -3421,9 +3556,7 @@
       <c r="AB7" s="11"/>
       <c r="AC7" s="11"/>
       <c r="AD7" s="11"/>
-      <c r="AE7" s="18">
-        <v>1</v>
-      </c>
+      <c r="AE7" s="11"/>
       <c r="AF7" s="11"/>
       <c r="AG7" s="11"/>
       <c r="AH7" s="11"/>
@@ -3442,92 +3575,549 @@
       <c r="AU7" s="11"/>
       <c r="AV7" s="11"/>
       <c r="AW7" s="11"/>
-      <c r="AX7" s="11"/>
-      <c r="AY7" s="2" t="s">
+      <c r="AX7" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="BA7" s="2">
+      <c r="AZ7" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>65</v>
       </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="B8" t="s">
         <v>66</v>
       </c>
+      <c r="C8" s="10" t="s">
+        <v>67</v>
+      </c>
       <c r="D8" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="E8" s="10" t="s">
         <v>63</v>
       </c>
+      <c r="E8" s="16">
+        <v>2</v>
+      </c>
       <c r="F8" s="16">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G8" s="16">
         <v>0</v>
       </c>
       <c r="H8" s="16">
+        <v>1</v>
+      </c>
+      <c r="I8" s="16">
         <v>0</v>
       </c>
-      <c r="I8" s="16">
+      <c r="K8" s="16">
+        <v>0</v>
+      </c>
+      <c r="L8" s="16">
         <v>1</v>
-      </c>
-      <c r="J8" s="16">
-        <v>0</v>
-      </c>
-      <c r="L8" s="16">
-        <v>0</v>
       </c>
       <c r="M8" s="16">
         <v>1</v>
       </c>
-      <c r="N8" s="16">
-        <v>1</v>
-      </c>
-      <c r="AE8" s="16">
-        <v>1</v>
-      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D4:AD4"/>
+    <mergeCell ref="C4:AD4"/>
   </mergeCells>
-  <dataValidations count="17">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AO7:AP7 AU7:AW7">
+  <dataValidations count="19">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showErrorMessage="1" sqref="S7:T1048576">
+      <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showErrorMessage="1" sqref="AD7:AD1048576 AB7:AB1048576">
+      <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation type="list" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W7:W1048576">
+      <formula1>date_choices</formula1>
+    </dataValidation>
+    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="P7:P1048576">
+      <formula1>validation_choices</formula1>
+    </dataValidation>
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O7:O1048576">
+      <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F7:I1048576 U7:V1048576 R7:R1048576 K7:M1048576">
+      <formula1>boolean_choices</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q7">
       <formula1>ouinon</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AL7">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showErrorMessage="1" sqref="E7">
       <formula1>0</formula1>
-      <formula2>200</formula2>
+      <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM7">
-      <formula1>validation_type</formula1>
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AP7 AR7">
+      <formula1>0</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AG7">
+      <formula1>datetype</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation type="list" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AF7">
+      <formula1>ouinon</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X7">
       <formula1>$S$7</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AG7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AL7">
+      <formula1>validation_type</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AK7">
+      <formula1>0</formula1>
+      <formula2>200</formula2>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AN7:AO7 AT7:AV7">
       <formula1>ouinon</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AC7">
-      <formula1>#REF!</formula1>
+    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="C7:C1048576">
+      <formula1>attribute_types</formula1>
+    </dataValidation>
+    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="D7:D1048576">
+      <formula1>attribute_groups</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z7:Z1048576">
+      <formula1>metric_types</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA7:AA1048576">
+      <formula1>metric_units</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:BC8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="Z1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="AE11" sqref="AE11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.7109375"/>
+    <col min="2" max="3" width="24.7109375"/>
+    <col min="4" max="4" width="23.7109375"/>
+    <col min="5" max="5" width="16.7109375"/>
+    <col min="6" max="6" width="19.7109375" style="16"/>
+    <col min="7" max="7" width="14" style="16"/>
+    <col min="8" max="8" width="13" style="16"/>
+    <col min="9" max="9" width="25.85546875" style="16"/>
+    <col min="10" max="10" width="25.140625" style="16"/>
+    <col min="11" max="11" width="20"/>
+    <col min="12" max="12" width="23.5703125" style="16"/>
+    <col min="13" max="13" width="23.85546875" style="16"/>
+    <col min="14" max="14" width="20.7109375" style="16"/>
+    <col min="15" max="15" width="13" style="16" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.42578125"/>
+    <col min="17" max="17" width="19.28515625"/>
+    <col min="18" max="19" width="17.28515625"/>
+    <col min="20" max="20" width="16.5703125"/>
+    <col min="21" max="21" width="19"/>
+    <col min="22" max="23" width="18.7109375"/>
+    <col min="24" max="25" width="13.42578125"/>
+    <col min="26" max="26" width="19.85546875"/>
+    <col min="27" max="27" width="13.42578125"/>
+    <col min="28" max="28" width="18.140625"/>
+    <col min="29" max="29" width="21"/>
+    <col min="30" max="30" width="22"/>
+    <col min="31" max="31" width="23.42578125"/>
+    <col min="32" max="32" width="14.85546875" style="16"/>
+    <col min="33" max="41" width="13.42578125"/>
+    <col min="42" max="42" width="16.85546875"/>
+    <col min="43" max="43" width="19.140625"/>
+    <col min="44" max="44" width="16.28515625"/>
+    <col min="45" max="47" width="13.42578125"/>
+    <col min="48" max="48" width="19.140625"/>
+    <col min="49" max="51" width="18.140625"/>
+    <col min="52" max="52" width="0" style="2" hidden="1"/>
+    <col min="53" max="53" width="0" style="3" hidden="1"/>
+    <col min="54" max="54" width="0" style="2" hidden="1"/>
+    <col min="55" max="55" width="17.140625" style="2"/>
+    <col min="56" max="1026" width="17.140625"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:55" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D1" s="4"/>
+      <c r="E1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AZ1"/>
+      <c r="BA1"/>
+      <c r="BB1"/>
+      <c r="BC1"/>
+    </row>
+    <row r="2" spans="1:55" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="AZ2"/>
+      <c r="BA2"/>
+      <c r="BB2"/>
+      <c r="BC2"/>
+    </row>
+    <row r="4" spans="1:55" s="19" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="25"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="31"/>
+      <c r="K4" s="31"/>
+      <c r="L4" s="31"/>
+      <c r="M4" s="31"/>
+      <c r="N4" s="31"/>
+      <c r="O4" s="31"/>
+      <c r="P4" s="31"/>
+      <c r="Q4" s="31"/>
+      <c r="R4" s="31"/>
+      <c r="S4" s="31"/>
+      <c r="T4" s="31"/>
+      <c r="U4" s="31"/>
+      <c r="V4" s="31"/>
+      <c r="W4" s="31"/>
+      <c r="X4" s="31"/>
+      <c r="Y4" s="31"/>
+      <c r="Z4" s="31"/>
+      <c r="AA4" s="31"/>
+      <c r="AB4" s="31"/>
+      <c r="AC4" s="31"/>
+      <c r="AD4" s="31"/>
+      <c r="AE4" s="31"/>
+      <c r="AF4" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:55" s="19" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="26" t="s">
+        <v>238</v>
+      </c>
+      <c r="H5" s="26" t="s">
+        <v>239</v>
+      </c>
+      <c r="I5" s="26" t="s">
+        <v>240</v>
+      </c>
+      <c r="J5" s="26" t="s">
+        <v>241</v>
+      </c>
+      <c r="K5" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="L5" s="26" t="s">
+        <v>242</v>
+      </c>
+      <c r="M5" s="26" t="s">
+        <v>243</v>
+      </c>
+      <c r="N5" s="26" t="s">
+        <v>244</v>
+      </c>
+      <c r="O5" s="26" t="s">
+        <v>268</v>
+      </c>
+      <c r="P5" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q5" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="R5" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="S5" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="T5" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="U5" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="V5" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="W5" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="X5" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y5" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z5" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA5" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB5" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC5" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD5" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE5" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF5" s="30" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:55" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="G6" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="H6" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="I6" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="J6" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="K6" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="L6" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="M6" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="N6" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="O6" s="17" t="s">
+        <v>269</v>
+      </c>
+      <c r="P6" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q6" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="R6" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="S6" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="T6" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="U6" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="V6" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="W6" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="X6" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="Y6" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="Z6" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA6" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB6" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC6" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="AD6" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE6" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="AF6" s="20"/>
+      <c r="AZ6"/>
+      <c r="BA6"/>
+      <c r="BB6"/>
+      <c r="BC6"/>
+    </row>
+    <row r="7" spans="1:55" x14ac:dyDescent="0.2">
+      <c r="A7" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="18"/>
+      <c r="M7" s="18"/>
+      <c r="N7" s="18"/>
+      <c r="O7" s="18"/>
+      <c r="P7" s="11"/>
+      <c r="R7" s="11"/>
+      <c r="S7" s="11"/>
+      <c r="T7" s="11"/>
+      <c r="U7" s="11"/>
+      <c r="V7" s="11"/>
+      <c r="W7" s="11"/>
+      <c r="X7" s="11"/>
+      <c r="Y7" s="11"/>
+      <c r="Z7" s="11"/>
+      <c r="AA7" s="11"/>
+      <c r="AB7" s="11"/>
+      <c r="AC7" s="11"/>
+      <c r="AD7" s="11"/>
+      <c r="AE7" s="11"/>
+      <c r="AF7" s="18">
+        <v>1</v>
+      </c>
+      <c r="AG7" s="11"/>
+      <c r="AH7" s="11"/>
+      <c r="AI7" s="11"/>
+      <c r="AJ7" s="11"/>
+      <c r="AK7" s="11"/>
+      <c r="AL7" s="11"/>
+      <c r="AM7" s="11"/>
+      <c r="AN7" s="11"/>
+      <c r="AO7" s="11"/>
+      <c r="AP7" s="11"/>
+      <c r="AQ7" s="11"/>
+      <c r="AR7" s="11"/>
+      <c r="AS7" s="11"/>
+      <c r="AT7" s="11"/>
+      <c r="AU7" s="11"/>
+      <c r="AV7" s="11"/>
+      <c r="AW7" s="11"/>
+      <c r="AX7" s="11"/>
+      <c r="AY7" s="11"/>
+      <c r="AZ7" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="BB7" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:55" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="AF8" s="16">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D4:AE4"/>
+  </mergeCells>
+  <dataValidations count="20">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AP7:AQ7 AV7:AX7">
+      <formula1>ouinon</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AH7">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM7">
+      <formula1>0</formula1>
+      <formula2>200</formula2>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AN7">
+      <formula1>validation_type</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y7">
+      <formula1>$T$7</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation type="list" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AH7">
+      <formula1>ouinon</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AI7">
       <formula1>datetype</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AQ7 AS7">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AR7 AT7">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -3535,72 +4125,56 @@
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q7">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R7">
       <formula1>ouinon</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G7:J1048576 L7:N1048576 R7:R1048576 B7:B1048576 U7:V1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G7:J1048576 V7:W1048576 S7:S1048576 B7:B1048576 L7:N1048576">
       <formula1>boolean_choices</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O7:O1048576">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P7:P1048576">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="P7:P1048576">
+    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="Q7:Q1048576">
       <formula1>validation_choices</formula1>
     </dataValidation>
-    <dataValidation operator="equal" allowBlank="1" showErrorMessage="1" sqref="S7:T1048576"/>
-    <dataValidation type="list" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W7:W1048576">
+    <dataValidation type="list" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X7:X1048576">
       <formula1>date_choices</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showErrorMessage="1" sqref="AD7:AD1048576 AB7:AB1048576">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showErrorMessage="1" sqref="AE7:AE1048576 AC7:AC1048576">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="AE7:AE1048576">
+    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="AF7:AF1048576">
       <formula1>boolean_choices</formula1>
+    </dataValidation>
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showErrorMessage="1" sqref="T7:U1048576">
+      <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="D1:D1048576">
+      <formula1>attribute_types</formula1>
+    </dataValidation>
+    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="E1:E1048576">
+      <formula1>attribute_groups</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA1:AA1048576">
+      <formula1>metric_types</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AB1:AB1048576">
+      <formula1>metric_units</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
-        <x14:dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>attribute_groups!$A$4:$A$257</xm:f>
-          </x14:formula1>
-          <xm:sqref>E7:E1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>metric_types!$B$3:$B$11</xm:f>
-          </x14:formula1>
-          <xm:sqref>Z7:Z1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>metric_units!$B$3:$B$89</xm:f>
-          </x14:formula1>
-          <xm:sqref>AA7:AA1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>attribute_types!$B$3:$B$14</xm:f>
-          </x14:formula1>
-          <xm:sqref>D7:D1048576</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView topLeftCell="A4" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3662,7 +4236,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -3732,12 +4306,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection sqref="A1:E1"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3827,7 +4401,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
@@ -3897,7 +4471,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -3963,13 +4537,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
-    </sheetView>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4043,49 +4615,4 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>212</v>
-      </c>
-      <c r="C1" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>213</v>
-      </c>
-      <c r="C2" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B3" t="s">
-        <v>214</v>
-      </c>
-      <c r="C3" t="s">
-        <v>217</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Removed required column on attributes tab
</commit_message>
<xml_diff>
--- a/Resources/fixtures/minimal/init.xlsx
+++ b/Resources/fixtures/minimal/init.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="6990" tabRatio="226" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="6990" tabRatio="226" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="10" r:id="rId1"/>
@@ -23,8 +23,8 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3">attribute_groups!$A$4:$C$4</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1">attributes!$B$6:$AZ$9</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2">'family main'!$C$6:$BB$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1">attributes!$B$6:$AY$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2">'family main'!$C$6:$BA$9</definedName>
     <definedName name="attribute_groups">attribute_groups!$A$4:$A$100</definedName>
     <definedName name="attribute_types">attribute_types!$B$3:$B$14</definedName>
     <definedName name="boolean_choices">choices!$A$1:$A$2</definedName>
@@ -43,6 +43,73 @@
     <author>SMILE</author>
   </authors>
   <commentList>
+    <comment ref="I5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Insert the name of the locales, separated by ",".
+For example : "en_US, fr_FR"
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AB5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Insert the allowed extensions, separated by a comma.
+For example : 
+jpg, jpeg, png</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AC5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Determines how many characters should be typed for select attributes before an option is presented.
+This should be used for attributes which have a large number of options.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>SMILE</author>
+  </authors>
+  <commentList>
+    <comment ref="AE4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Set to 1 if the attribute is required in this family for the concerned channel.</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="J5" authorId="0">
       <text>
         <r>
@@ -74,73 +141,6 @@
       </text>
     </comment>
     <comment ref="AD5" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Determines how many characters should be typed for select attributes before an option is presented.
-This should be used for attributes which have a large number of options.</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>SMILE</author>
-  </authors>
-  <commentList>
-    <comment ref="AF4" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Set to 1 if the attribute is required in this family for the concerned channel.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="K5" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Insert the name of the locales, separated by ",".
-For example : "en_US, fr_FR"
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AD5" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Insert the allowed extensions, separated by a comma.
-For example : 
-jpg, jpeg, png</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AE5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -220,7 +220,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="272">
   <si>
     <t>en_US</t>
   </si>
@@ -328,9 +328,6 @@
   </si>
   <si>
     <t>sort_order</t>
-  </si>
-  <si>
-    <t>required</t>
   </si>
   <si>
     <t>unique</t>
@@ -1022,9 +1019,6 @@
       </rPr>
       <t>All category tabs should start with "categories"</t>
     </r>
-  </si>
-  <si>
-    <t>Is required*</t>
   </si>
   <si>
     <t>Is unique*</t>
@@ -2012,32 +2006,32 @@
   <sheetData>
     <row r="1" spans="1:2" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A1" s="22" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="21" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B5" s="23" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B6" s="24" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B7" s="24" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B8" s="24" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -2045,7 +2039,7 @@
     </row>
     <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="21" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -2053,127 +2047,127 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B12" s="23" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B15" s="21" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="22" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B22" s="21" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="26" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B26" s="21" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="29" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="31" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B31" s="21" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B34" s="24" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="36" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B36" s="21" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="38" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="39" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="41" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B41" s="21" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="43" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="45" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B45" s="21" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="47" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A50" s="29" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B52" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
   </sheetData>
@@ -2197,10 +2191,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -2208,18 +2202,18 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
   </sheetData>
@@ -2244,10 +2238,10 @@
   <sheetData>
     <row r="1" spans="1:2" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>110</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -2255,103 +2249,103 @@
         <v>30</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>113</v>
+      </c>
+      <c r="B5" t="s">
         <v>114</v>
-      </c>
-      <c r="B5" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>115</v>
+      </c>
+      <c r="B6" t="s">
         <v>116</v>
-      </c>
-      <c r="B6" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>117</v>
+      </c>
+      <c r="B7" t="s">
         <v>118</v>
-      </c>
-      <c r="B7" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>119</v>
+      </c>
+      <c r="B8" t="s">
         <v>120</v>
-      </c>
-      <c r="B8" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>121</v>
+      </c>
+      <c r="B9" t="s">
         <v>122</v>
-      </c>
-      <c r="B9" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>123</v>
+      </c>
+      <c r="B10" t="s">
         <v>124</v>
-      </c>
-      <c r="B10" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>125</v>
+      </c>
+      <c r="B11" t="s">
         <v>126</v>
-      </c>
-      <c r="B11" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>127</v>
+      </c>
+      <c r="B12" t="s">
         <v>128</v>
-      </c>
-      <c r="B12" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>129</v>
+      </c>
+      <c r="B13" t="s">
         <v>130</v>
-      </c>
-      <c r="B13" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>131</v>
+      </c>
+      <c r="B14" t="s">
         <v>132</v>
-      </c>
-      <c r="B14" t="s">
-        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -2381,10 +2375,10 @@
   <sheetData>
     <row r="1" spans="1:2" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>110</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -2392,79 +2386,79 @@
         <v>30</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -2494,7 +2488,7 @@
   <sheetData>
     <row r="1" spans="1:1024" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B1" s="9"/>
       <c r="AMJ1"/>
@@ -2504,704 +2498,704 @@
         <v>33</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="AMJ2"/>
     </row>
     <row r="3" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="4" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="5" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="6" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="7" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="8" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="9" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="10" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B10" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="11" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B11" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="12" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B12" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="13" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B13" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="14" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B14" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="15" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B15" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="16" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B16" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B17" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B18" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B19" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B20" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B21" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B22" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B23" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B24" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B25" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B26" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B27" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B28" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B29" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B30" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B31" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B32" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B33" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B34" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B35" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B36" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B37" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B38" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B39" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B40" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B41" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B42" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B43" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B44" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B45" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B46" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B47" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B48" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B49" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B50" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B51" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B52" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B53" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B54" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B55" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B56" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B57" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B58" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B59" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B60" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B61" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B62" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B63" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B64" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B65" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B66" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B67" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B68" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B69" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B70" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B71" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B72" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B73" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B74" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B75" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B76" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B77" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B78" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B79" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B80" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B81" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B82" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B83" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B84" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B85" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B86" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B87" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B88" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B89" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
   </sheetData>
@@ -3216,10 +3210,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BA8"/>
+  <dimension ref="A1:AZ8"/>
   <sheetViews>
-    <sheetView topLeftCell="V1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="AA15" sqref="AA15"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3229,56 +3223,55 @@
     <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.85546875" style="16" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" style="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.85546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.7109375" style="16" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23.42578125" style="16" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.5703125" style="16" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.28515625" style="16" customWidth="1"/>
-    <col min="15" max="15" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="17" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="14" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="19" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="21" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="9.140625" style="2"/>
-    <col min="51" max="51" width="9.140625" style="3"/>
-    <col min="52" max="53" width="9.140625" style="2"/>
+    <col min="6" max="6" width="10.140625" style="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" style="16" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" style="16" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.140625" style="16" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.42578125" style="16" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.5703125" style="16" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.28515625" style="16" customWidth="1"/>
+    <col min="14" max="14" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="17" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="19" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="9.140625" style="2"/>
+    <col min="50" max="50" width="9.140625" style="3"/>
+    <col min="51" max="52" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:52" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="24" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
+      <c r="AW1"/>
       <c r="AX1"/>
       <c r="AY1"/>
       <c r="AZ1"/>
-      <c r="BA1"/>
-    </row>
-    <row r="2" spans="1:53" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:52" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4"/>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
+      <c r="AW2"/>
       <c r="AX2"/>
       <c r="AY2"/>
       <c r="AZ2"/>
-      <c r="BA2"/>
-    </row>
-    <row r="4" spans="1:53" s="19" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:52" s="19" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="25"/>
       <c r="B4" s="6" t="s">
         <v>5</v>
@@ -3312,9 +3305,8 @@
       <c r="AA4" s="31"/>
       <c r="AB4" s="31"/>
       <c r="AC4" s="31"/>
-      <c r="AD4" s="31"/>
-    </row>
-    <row r="5" spans="1:53" s="19" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:52" s="19" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="25" t="s">
         <v>8</v>
       </c>
@@ -3331,82 +3323,79 @@
         <v>12</v>
       </c>
       <c r="F5" s="26" t="s">
+        <v>237</v>
+      </c>
+      <c r="G5" s="26" t="s">
         <v>238</v>
       </c>
-      <c r="G5" s="26" t="s">
+      <c r="H5" s="26" t="s">
         <v>239</v>
       </c>
-      <c r="H5" s="26" t="s">
+      <c r="I5" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="J5" s="26" t="s">
         <v>240</v>
       </c>
-      <c r="I5" s="26" t="s">
+      <c r="K5" s="26" t="s">
         <v>241</v>
       </c>
-      <c r="J5" s="26" t="s">
-        <v>13</v>
-      </c>
-      <c r="K5" s="26" t="s">
+      <c r="L5" s="26" t="s">
         <v>242</v>
       </c>
-      <c r="L5" s="26" t="s">
-        <v>243</v>
-      </c>
       <c r="M5" s="26" t="s">
-        <v>244</v>
+        <v>266</v>
       </c>
       <c r="N5" s="26" t="s">
-        <v>268</v>
+        <v>14</v>
       </c>
       <c r="O5" s="26" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="P5" s="26" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="Q5" s="26" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="R5" s="26" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="S5" s="26" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="T5" s="26" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="U5" s="26" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="V5" s="26" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="W5" s="26" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="X5" s="26" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="Y5" s="26" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Z5" s="26" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="AA5" s="26" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="AB5" s="26" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="AC5" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="AD5" s="26" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:53" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:52" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>30</v>
       </c>
@@ -3431,10 +3420,10 @@
       <c r="H6" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="I6" s="17" t="s">
+      <c r="I6" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="J6" s="9" t="s">
+      <c r="J6" s="17" t="s">
         <v>40</v>
       </c>
       <c r="K6" s="17" t="s">
@@ -3444,10 +3433,10 @@
         <v>42</v>
       </c>
       <c r="M6" s="17" t="s">
+        <v>267</v>
+      </c>
+      <c r="N6" s="9" t="s">
         <v>43</v>
-      </c>
-      <c r="N6" s="17" t="s">
-        <v>269</v>
       </c>
       <c r="O6" s="9" t="s">
         <v>44</v>
@@ -3494,54 +3483,49 @@
       <c r="AC6" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="AD6" s="9" t="s">
-        <v>59</v>
-      </c>
+      <c r="AW6"/>
       <c r="AX6"/>
       <c r="AY6"/>
       <c r="AZ6"/>
-      <c r="BA6"/>
-    </row>
-    <row r="7" spans="1:53" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7" t="s">
         <v>60</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="D7" s="10" t="s">
         <v>62</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>63</v>
       </c>
       <c r="E7" s="16">
         <v>1</v>
       </c>
       <c r="F7" s="18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G7" s="18">
         <v>1</v>
       </c>
       <c r="H7" s="18">
+        <v>0</v>
+      </c>
+      <c r="I7" s="11"/>
+      <c r="J7" s="18">
+        <v>0</v>
+      </c>
+      <c r="K7" s="18">
         <v>1</v>
-      </c>
-      <c r="I7" s="18">
-        <v>0</v>
-      </c>
-      <c r="J7" s="11"/>
-      <c r="K7" s="18">
-        <v>0</v>
       </c>
       <c r="L7" s="18">
         <v>1</v>
       </c>
-      <c r="M7" s="18">
-        <v>1</v>
-      </c>
-      <c r="N7" s="18"/>
-      <c r="O7" s="11"/>
+      <c r="M7" s="18"/>
+      <c r="N7" s="11"/>
+      <c r="P7" s="11"/>
       <c r="Q7" s="11"/>
       <c r="R7" s="11"/>
       <c r="S7" s="11"/>
@@ -3574,26 +3558,25 @@
       <c r="AT7" s="11"/>
       <c r="AU7" s="11"/>
       <c r="AV7" s="11"/>
-      <c r="AW7" s="11"/>
-      <c r="AX7" s="2" t="s">
+      <c r="AW7" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="AY7" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:52" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>64</v>
       </c>
-      <c r="AZ7" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="B8" t="s">
         <v>65</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="C8" s="10" t="s">
-        <v>67</v>
-      </c>
       <c r="D8" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E8" s="16">
         <v>2</v>
@@ -3602,48 +3585,45 @@
         <v>0</v>
       </c>
       <c r="G8" s="16">
+        <v>1</v>
+      </c>
+      <c r="H8" s="16">
         <v>0</v>
       </c>
-      <c r="H8" s="16">
+      <c r="J8" s="16">
+        <v>0</v>
+      </c>
+      <c r="K8" s="16">
         <v>1</v>
-      </c>
-      <c r="I8" s="16">
-        <v>0</v>
-      </c>
-      <c r="K8" s="16">
-        <v>0</v>
       </c>
       <c r="L8" s="16">
         <v>1</v>
       </c>
-      <c r="M8" s="16">
-        <v>1</v>
-      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="C4:AD4"/>
+    <mergeCell ref="C4:AC4"/>
   </mergeCells>
   <dataValidations count="19">
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showErrorMessage="1" sqref="S7:T1048576">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showErrorMessage="1" sqref="R7:S1048576">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showErrorMessage="1" sqref="AD7:AD1048576 AB7:AB1048576">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showErrorMessage="1" sqref="AC7:AC1048576 AA7:AA1048576">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="list" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W7:W1048576">
+    <dataValidation type="list" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V7:V1048576">
       <formula1>date_choices</formula1>
     </dataValidation>
-    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="P7:P1048576">
+    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="O7:O1048576">
       <formula1>validation_choices</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O7:O1048576">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N7:N1048576">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F7:I1048576 U7:V1048576 R7:R1048576 K7:M1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T7:U1048576 Q7:Q1048576 J7:L1048576 F7:H1048576">
       <formula1>boolean_choices</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q7">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P7">
       <formula1>ouinon</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -3651,31 +3631,31 @@
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AP7 AR7">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AO7 AQ7">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AG7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AF7">
       <formula1>datetype</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AF7">
+    <dataValidation type="list" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AE7">
       <formula1>ouinon</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X7">
-      <formula1>$S$7</formula1>
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W7">
+      <formula1>$R$7</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AL7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AK7">
       <formula1>validation_type</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AK7">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AJ7">
       <formula1>0</formula1>
       <formula2>200</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AN7:AO7 AT7:AV7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM7:AN7 AS7:AU7">
       <formula1>ouinon</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -3685,10 +3665,10 @@
     <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="D7:D1048576">
       <formula1>attribute_groups</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z7:Z1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y7:Y1048576">
       <formula1>metric_types</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA7:AA1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z7:Z1048576">
       <formula1>metric_units</formula1>
     </dataValidation>
   </dataValidations>
@@ -3700,10 +3680,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BC8"/>
+  <dimension ref="A1:BB8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Z1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="AE11" sqref="AE11"/>
+    <sheetView topLeftCell="D1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3713,54 +3693,53 @@
     <col min="4" max="4" width="23.7109375"/>
     <col min="5" max="5" width="16.7109375"/>
     <col min="6" max="6" width="19.7109375" style="16"/>
-    <col min="7" max="7" width="14" style="16"/>
-    <col min="8" max="8" width="13" style="16"/>
-    <col min="9" max="9" width="25.85546875" style="16"/>
-    <col min="10" max="10" width="25.140625" style="16"/>
-    <col min="11" max="11" width="20"/>
-    <col min="12" max="12" width="23.5703125" style="16"/>
-    <col min="13" max="13" width="23.85546875" style="16"/>
-    <col min="14" max="14" width="20.7109375" style="16"/>
-    <col min="15" max="15" width="13" style="16" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20.42578125"/>
-    <col min="17" max="17" width="19.28515625"/>
-    <col min="18" max="19" width="17.28515625"/>
-    <col min="20" max="20" width="16.5703125"/>
-    <col min="21" max="21" width="19"/>
-    <col min="22" max="23" width="18.7109375"/>
-    <col min="24" max="25" width="13.42578125"/>
-    <col min="26" max="26" width="19.85546875"/>
-    <col min="27" max="27" width="13.42578125"/>
-    <col min="28" max="28" width="18.140625"/>
-    <col min="29" max="29" width="21"/>
-    <col min="30" max="30" width="22"/>
-    <col min="31" max="31" width="23.42578125"/>
-    <col min="32" max="32" width="14.85546875" style="16"/>
-    <col min="33" max="41" width="13.42578125"/>
-    <col min="42" max="42" width="16.85546875"/>
-    <col min="43" max="43" width="19.140625"/>
-    <col min="44" max="44" width="16.28515625"/>
-    <col min="45" max="47" width="13.42578125"/>
-    <col min="48" max="48" width="19.140625"/>
-    <col min="49" max="51" width="18.140625"/>
-    <col min="52" max="52" width="0" style="2" hidden="1"/>
-    <col min="53" max="53" width="0" style="3" hidden="1"/>
-    <col min="54" max="54" width="0" style="2" hidden="1"/>
-    <col min="55" max="55" width="17.140625" style="2"/>
-    <col min="56" max="1026" width="17.140625"/>
+    <col min="7" max="7" width="13" style="16"/>
+    <col min="8" max="8" width="25.85546875" style="16"/>
+    <col min="9" max="9" width="25.140625" style="16"/>
+    <col min="10" max="10" width="20"/>
+    <col min="11" max="11" width="23.5703125" style="16"/>
+    <col min="12" max="12" width="23.85546875" style="16"/>
+    <col min="13" max="13" width="20.7109375" style="16"/>
+    <col min="14" max="14" width="13" style="16" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20.42578125"/>
+    <col min="16" max="16" width="19.28515625"/>
+    <col min="17" max="18" width="17.28515625"/>
+    <col min="19" max="19" width="16.5703125"/>
+    <col min="20" max="20" width="19"/>
+    <col min="21" max="22" width="18.7109375"/>
+    <col min="23" max="24" width="13.42578125"/>
+    <col min="25" max="25" width="19.85546875"/>
+    <col min="26" max="26" width="13.42578125"/>
+    <col min="27" max="27" width="18.140625"/>
+    <col min="28" max="28" width="21"/>
+    <col min="29" max="29" width="22"/>
+    <col min="30" max="30" width="23.42578125"/>
+    <col min="31" max="31" width="14.85546875" style="16"/>
+    <col min="32" max="40" width="13.42578125"/>
+    <col min="41" max="41" width="16.85546875"/>
+    <col min="42" max="42" width="19.140625"/>
+    <col min="43" max="43" width="16.28515625"/>
+    <col min="44" max="46" width="13.42578125"/>
+    <col min="47" max="47" width="19.140625"/>
+    <col min="48" max="50" width="18.140625"/>
+    <col min="51" max="51" width="0" style="2" hidden="1"/>
+    <col min="52" max="52" width="0" style="3" hidden="1"/>
+    <col min="53" max="53" width="0" style="2" hidden="1"/>
+    <col min="54" max="54" width="17.140625" style="2"/>
+    <col min="55" max="1025" width="17.140625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:55" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:54" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D1" s="4"/>
       <c r="E1" s="4" t="s">
         <v>0</v>
       </c>
+      <c r="AY1"/>
       <c r="AZ1"/>
       <c r="BA1"/>
       <c r="BB1"/>
-      <c r="BC1"/>
-    </row>
-    <row r="2" spans="1:55" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:54" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -3773,12 +3752,12 @@
       <c r="E2" s="4" t="s">
         <v>4</v>
       </c>
+      <c r="AY2"/>
       <c r="AZ2"/>
       <c r="BA2"/>
       <c r="BB2"/>
-      <c r="BC2"/>
-    </row>
-    <row r="4" spans="1:55" s="19" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:54" s="19" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="25"/>
       <c r="B4" s="25"/>
       <c r="C4" s="6" t="s">
@@ -3813,12 +3792,11 @@
       <c r="AB4" s="31"/>
       <c r="AC4" s="31"/>
       <c r="AD4" s="31"/>
-      <c r="AE4" s="31"/>
-      <c r="AF4" s="7" t="s">
+      <c r="AE4" s="7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:55" s="19" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:54" s="19" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="25" t="s">
         <v>8</v>
       </c>
@@ -3838,85 +3816,82 @@
         <v>12</v>
       </c>
       <c r="G5" s="26" t="s">
+        <v>237</v>
+      </c>
+      <c r="H5" s="26" t="s">
         <v>238</v>
       </c>
-      <c r="H5" s="26" t="s">
+      <c r="I5" s="26" t="s">
         <v>239</v>
       </c>
-      <c r="I5" s="26" t="s">
+      <c r="J5" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="K5" s="26" t="s">
         <v>240</v>
       </c>
-      <c r="J5" s="26" t="s">
+      <c r="L5" s="26" t="s">
         <v>241</v>
       </c>
-      <c r="K5" s="26" t="s">
-        <v>13</v>
-      </c>
-      <c r="L5" s="26" t="s">
+      <c r="M5" s="26" t="s">
         <v>242</v>
       </c>
-      <c r="M5" s="26" t="s">
-        <v>243</v>
-      </c>
       <c r="N5" s="26" t="s">
-        <v>244</v>
+        <v>266</v>
       </c>
       <c r="O5" s="26" t="s">
-        <v>268</v>
+        <v>14</v>
       </c>
       <c r="P5" s="26" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="Q5" s="26" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="R5" s="26" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="S5" s="26" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="T5" s="26" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="U5" s="26" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="V5" s="26" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="W5" s="26" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="X5" s="26" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="Y5" s="26" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="Z5" s="26" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="AA5" s="26" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="AB5" s="26" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="AC5" s="26" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="AD5" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="AE5" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="AF5" s="30" t="s">
+      <c r="AE5" s="30" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:55" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:54" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>30</v>
       </c>
@@ -3944,10 +3919,10 @@
       <c r="I6" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="J6" s="17" t="s">
+      <c r="J6" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="K6" s="9" t="s">
+      <c r="K6" s="17" t="s">
         <v>40</v>
       </c>
       <c r="L6" s="17" t="s">
@@ -3957,10 +3932,10 @@
         <v>42</v>
       </c>
       <c r="N6" s="17" t="s">
+        <v>267</v>
+      </c>
+      <c r="O6" s="9" t="s">
         <v>43</v>
-      </c>
-      <c r="O6" s="17" t="s">
-        <v>269</v>
       </c>
       <c r="P6" s="9" t="s">
         <v>44</v>
@@ -4007,31 +3982,28 @@
       <c r="AD6" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="AE6" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="AF6" s="20"/>
+      <c r="AE6" s="20"/>
+      <c r="AY6"/>
       <c r="AZ6"/>
       <c r="BA6"/>
       <c r="BB6"/>
-      <c r="BC6"/>
-    </row>
-    <row r="7" spans="1:55" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
       <c r="G7" s="18"/>
       <c r="H7" s="18"/>
       <c r="I7" s="18"/>
-      <c r="J7" s="18"/>
-      <c r="K7" s="11"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="18"/>
       <c r="L7" s="18"/>
       <c r="M7" s="18"/>
       <c r="N7" s="18"/>
-      <c r="O7" s="18"/>
-      <c r="P7" s="11"/>
+      <c r="O7" s="11"/>
+      <c r="Q7" s="11"/>
       <c r="R7" s="11"/>
       <c r="S7" s="11"/>
       <c r="T7" s="11"/>
@@ -4045,10 +4017,10 @@
       <c r="AB7" s="11"/>
       <c r="AC7" s="11"/>
       <c r="AD7" s="11"/>
-      <c r="AE7" s="11"/>
-      <c r="AF7" s="18">
+      <c r="AE7" s="18">
         <v>1</v>
       </c>
+      <c r="AF7" s="11"/>
       <c r="AG7" s="11"/>
       <c r="AH7" s="11"/>
       <c r="AI7" s="11"/>
@@ -4067,57 +4039,56 @@
       <c r="AV7" s="11"/>
       <c r="AW7" s="11"/>
       <c r="AX7" s="11"/>
-      <c r="AY7" s="11"/>
-      <c r="AZ7" s="2" t="s">
+      <c r="AY7" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="BA7" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:54" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>64</v>
-      </c>
-      <c r="BB7" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:55" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>65</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>
-      <c r="AF8" s="16">
+      <c r="AE8" s="16">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D4:AE4"/>
+    <mergeCell ref="D4:AD4"/>
   </mergeCells>
   <dataValidations count="20">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AP7:AQ7 AV7:AX7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AO7:AP7 AU7:AW7">
       <formula1>ouinon</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM7">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AL7">
       <formula1>0</formula1>
       <formula2>200</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AN7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM7">
       <formula1>validation_type</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y7">
-      <formula1>$T$7</formula1>
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X7">
+      <formula1>$S$7</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AH7">
+    <dataValidation type="list" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AG7">
       <formula1>ouinon</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AI7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AH7">
       <formula1>datetype</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AR7 AT7">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AQ7 AS7">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -4125,29 +4096,29 @@
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R7">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q7">
       <formula1>ouinon</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G7:J1048576 V7:W1048576 S7:S1048576 B7:B1048576 L7:N1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U7:V1048576 R7:R1048576 B7:B1048576 K7:M1048576 G7:I1048576">
       <formula1>boolean_choices</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P7:P1048576">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O7:O1048576">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="Q7:Q1048576">
+    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="P7:P1048576">
       <formula1>validation_choices</formula1>
     </dataValidation>
-    <dataValidation type="list" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X7:X1048576">
+    <dataValidation type="list" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W7:W1048576">
       <formula1>date_choices</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showErrorMessage="1" sqref="AE7:AE1048576 AC7:AC1048576">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showErrorMessage="1" sqref="AD7:AD1048576 AB7:AB1048576">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="AF7:AF1048576">
+    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="AE7:AE1048576">
       <formula1>boolean_choices</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showErrorMessage="1" sqref="T7:U1048576">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showErrorMessage="1" sqref="S7:T1048576">
       <formula1>0</formula1>
     </dataValidation>
     <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="D1:D1048576">
@@ -4156,10 +4127,10 @@
     <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="E1:E1048576">
       <formula1>attribute_groups</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA1:AA1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z1:Z1048576">
       <formula1>metric_types</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AB1:AB1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA1:AA1048576">
       <formula1>metric_units</formula1>
     </dataValidation>
   </dataValidations>
@@ -4187,7 +4158,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="32" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B1" s="32"/>
       <c r="C1" s="13" t="s">
@@ -4196,10 +4167,10 @@
     </row>
     <row r="2" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" s="9" t="s">
         <v>69</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>70</v>
       </c>
       <c r="C2" s="14" t="s">
         <v>0</v>
@@ -4218,13 +4189,13 @@
     </row>
     <row r="4" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B4" s="11">
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -4254,7 +4225,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="32" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B1" s="32"/>
       <c r="C1" s="32"/>
@@ -4267,10 +4238,10 @@
         <v>8</v>
       </c>
       <c r="B2" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C2" s="9" t="s">
         <v>73</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>74</v>
       </c>
       <c r="D2" s="14" t="s">
         <v>0</v>
@@ -4278,13 +4249,13 @@
     </row>
     <row r="3" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>30</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>32</v>
@@ -4326,7 +4297,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B1" s="32"/>
       <c r="C1" s="32"/>
@@ -4335,19 +4306,19 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="C2" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="D2" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="E2" s="9" t="s">
         <v>81</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
@@ -4355,16 +4326,16 @@
         <v>30</v>
       </c>
       <c r="B3" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="C3" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="D3" s="9" t="s">
+      <c r="E3" s="9" t="s">
         <v>93</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4378,7 +4349,7 @@
         <v>0</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E4" s="11" t="s">
         <v>2</v>
@@ -4418,7 +4389,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="32" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B1" s="32"/>
       <c r="C1" s="13" t="s">
@@ -4427,10 +4398,10 @@
     </row>
     <row r="2" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="B2" s="9" t="s">
         <v>106</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>107</v>
       </c>
       <c r="C2" s="14" t="s">
         <v>0</v>
@@ -4441,7 +4412,7 @@
         <v>30</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C3" s="14" t="s">
         <v>32</v>
@@ -4452,7 +4423,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -4487,7 +4458,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="32" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B1" s="32"/>
     </row>
@@ -4496,7 +4467,7 @@
         <v>30</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="3" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
@@ -4504,12 +4475,12 @@
         <v>30</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -4517,7 +4488,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -4551,7 +4522,7 @@
   <sheetData>
     <row r="1" spans="1:2" s="28" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>5</v>
@@ -4559,7 +4530,7 @@
     </row>
     <row r="2" spans="1:2" s="28" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="26" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B2" s="13" t="s">
         <v>0</v>
@@ -4575,34 +4546,34 @@
     </row>
     <row r="4" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B4" s="27" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B5" s="28" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B6" s="28" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B7" s="28" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added back the required column
</commit_message>
<xml_diff>
--- a/Resources/fixtures/minimal/init.xlsx
+++ b/Resources/fixtures/minimal/init.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="6990" tabRatio="226" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="6990" tabRatio="226" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="10" r:id="rId1"/>
@@ -23,8 +23,8 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3">attribute_groups!$A$4:$C$4</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1">attributes!$B$6:$AY$9</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2">'family main'!$C$6:$BA$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1">attributes!$B$6:$AZ$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2">'family main'!$C$6:$BB$9</definedName>
     <definedName name="attribute_groups">attribute_groups!$A$4:$A$100</definedName>
     <definedName name="attribute_types">attribute_types!$B$3:$B$14</definedName>
     <definedName name="boolean_choices">choices!$A$1:$A$2</definedName>
@@ -43,7 +43,7 @@
     <author>SMILE</author>
   </authors>
   <commentList>
-    <comment ref="I5" authorId="0">
+    <comment ref="F5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -52,61 +52,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">Insert the name of the locales, separated by ",".
-For example : "en_US, fr_FR"
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AB5" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Insert the allowed extensions, separated by a comma.
-For example : 
-jpg, jpeg, png</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AC5" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Determines how many characters should be typed for select attributes before an option is presented.
-This should be used for attributes which have a large number of options.</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>SMILE</author>
-  </authors>
-  <commentList>
-    <comment ref="AE4" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Set to 1 if the attribute is required in this family for the concerned channel.</t>
+          <t>The value must be 1 for the identifier, and must be 0 for all other attributes</t>
         </r>
       </text>
     </comment>
@@ -141,6 +87,86 @@
       </text>
     </comment>
     <comment ref="AD5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Determines how many characters should be typed for select attributes before an option is presented.
+This should be used for attributes which have a large number of options.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>SMILE</author>
+  </authors>
+  <commentList>
+    <comment ref="AF4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Set to 1 if the attribute is required in this family for the concerned channel.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The value must be 1 for the identifier, and must be 0 for all other attributes</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Insert the name of the locales, separated by ",".
+For example : "en_US, fr_FR"
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AD5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Insert the allowed extensions, separated by a comma.
+For example : 
+jpg, jpeg, png</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AE5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -220,7 +246,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="275">
   <si>
     <t>en_US</t>
   </si>
@@ -1147,6 +1173,15 @@
   </si>
   <si>
     <t>Common and unaffected attribute properties</t>
+  </si>
+  <si>
+    <t>Required *</t>
+  </si>
+  <si>
+    <t>required</t>
+  </si>
+  <si>
+    <t>Is required*</t>
   </si>
 </sst>
 </file>
@@ -1995,8 +2030,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B53"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:XFD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3210,10 +3245,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AZ8"/>
+  <dimension ref="A1:BA8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3223,55 +3258,56 @@
     <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.85546875" style="16" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.85546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.7109375" style="16" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.42578125" style="16" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.5703125" style="16" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.28515625" style="16" customWidth="1"/>
-    <col min="14" max="14" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="17" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="14" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="19" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="21" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="9.140625" style="2"/>
-    <col min="50" max="50" width="9.140625" style="3"/>
-    <col min="51" max="52" width="9.140625" style="2"/>
+    <col min="6" max="6" width="13.28515625" style="16" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" style="16" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.85546875" style="16" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" style="16" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" style="16" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23.42578125" style="16" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.5703125" style="16" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.28515625" style="16" customWidth="1"/>
+    <col min="15" max="15" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="17" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="14" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="19" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="21" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="9.140625" style="2"/>
+    <col min="51" max="51" width="9.140625" style="3"/>
+    <col min="52" max="53" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:52" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:53" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="24" t="s">
         <v>271</v>
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
-      <c r="AW1"/>
       <c r="AX1"/>
       <c r="AY1"/>
       <c r="AZ1"/>
-    </row>
-    <row r="2" spans="1:52" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BA1"/>
+    </row>
+    <row r="2" spans="1:53" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4"/>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
-      <c r="AW2"/>
       <c r="AX2"/>
       <c r="AY2"/>
       <c r="AZ2"/>
-    </row>
-    <row r="4" spans="1:52" s="19" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BA2"/>
+    </row>
+    <row r="4" spans="1:53" s="19" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="25"/>
       <c r="B4" s="6" t="s">
         <v>5</v>
@@ -3305,8 +3341,9 @@
       <c r="AA4" s="31"/>
       <c r="AB4" s="31"/>
       <c r="AC4" s="31"/>
-    </row>
-    <row r="5" spans="1:52" s="19" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AD4" s="31"/>
+    </row>
+    <row r="5" spans="1:53" s="19" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="25" t="s">
         <v>8</v>
       </c>
@@ -3323,79 +3360,82 @@
         <v>12</v>
       </c>
       <c r="F5" s="26" t="s">
+        <v>272</v>
+      </c>
+      <c r="G5" s="26" t="s">
         <v>237</v>
       </c>
-      <c r="G5" s="26" t="s">
+      <c r="H5" s="26" t="s">
         <v>238</v>
       </c>
-      <c r="H5" s="26" t="s">
+      <c r="I5" s="26" t="s">
         <v>239</v>
       </c>
-      <c r="I5" s="26" t="s">
+      <c r="J5" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="J5" s="26" t="s">
+      <c r="K5" s="26" t="s">
         <v>240</v>
       </c>
-      <c r="K5" s="26" t="s">
+      <c r="L5" s="26" t="s">
         <v>241</v>
       </c>
-      <c r="L5" s="26" t="s">
+      <c r="M5" s="26" t="s">
         <v>242</v>
       </c>
-      <c r="M5" s="26" t="s">
+      <c r="N5" s="26" t="s">
         <v>266</v>
       </c>
-      <c r="N5" s="26" t="s">
+      <c r="O5" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="O5" s="26" t="s">
+      <c r="P5" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="P5" s="26" t="s">
+      <c r="Q5" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="Q5" s="26" t="s">
+      <c r="R5" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="R5" s="26" t="s">
+      <c r="S5" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="S5" s="26" t="s">
+      <c r="T5" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="T5" s="26" t="s">
+      <c r="U5" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="U5" s="26" t="s">
+      <c r="V5" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="V5" s="26" t="s">
+      <c r="W5" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="W5" s="26" t="s">
+      <c r="X5" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="X5" s="26" t="s">
+      <c r="Y5" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="Y5" s="26" t="s">
+      <c r="Z5" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="Z5" s="26" t="s">
+      <c r="AA5" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="AA5" s="26" t="s">
+      <c r="AB5" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="AB5" s="26" t="s">
+      <c r="AC5" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="AC5" s="26" t="s">
+      <c r="AD5" s="26" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:52" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:53" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>30</v>
       </c>
@@ -3412,83 +3452,86 @@
         <v>35</v>
       </c>
       <c r="F6" s="17" t="s">
+        <v>273</v>
+      </c>
+      <c r="G6" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="G6" s="17" t="s">
+      <c r="H6" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="H6" s="17" t="s">
+      <c r="I6" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="I6" s="9" t="s">
+      <c r="J6" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="J6" s="17" t="s">
+      <c r="K6" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="K6" s="17" t="s">
+      <c r="L6" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="L6" s="17" t="s">
+      <c r="M6" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="M6" s="17" t="s">
+      <c r="N6" s="17" t="s">
         <v>267</v>
       </c>
-      <c r="N6" s="9" t="s">
+      <c r="O6" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="O6" s="9" t="s">
+      <c r="P6" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="P6" s="9" t="s">
+      <c r="Q6" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="Q6" s="9" t="s">
+      <c r="R6" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="R6" s="9" t="s">
+      <c r="S6" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="S6" s="9" t="s">
+      <c r="T6" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="T6" s="9" t="s">
+      <c r="U6" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="U6" s="9" t="s">
+      <c r="V6" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="V6" s="9" t="s">
+      <c r="W6" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="W6" s="9" t="s">
+      <c r="X6" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="X6" s="9" t="s">
+      <c r="Y6" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="Y6" s="9" t="s">
+      <c r="Z6" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="Z6" s="9" t="s">
+      <c r="AA6" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="AA6" s="9" t="s">
+      <c r="AB6" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="AB6" s="9" t="s">
+      <c r="AC6" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="AC6" s="9" t="s">
+      <c r="AD6" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="AW6"/>
       <c r="AX6"/>
       <c r="AY6"/>
       <c r="AZ6"/>
-    </row>
-    <row r="7" spans="1:52" x14ac:dyDescent="0.2">
+      <c r="BA6"/>
+    </row>
+    <row r="7" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
         <v>59</v>
       </c>
@@ -3511,21 +3554,23 @@
         <v>1</v>
       </c>
       <c r="H7" s="18">
+        <v>1</v>
+      </c>
+      <c r="I7" s="18">
         <v>0</v>
       </c>
-      <c r="I7" s="11"/>
-      <c r="J7" s="18">
+      <c r="J7" s="11"/>
+      <c r="K7" s="18">
         <v>0</v>
-      </c>
-      <c r="K7" s="18">
-        <v>1</v>
       </c>
       <c r="L7" s="18">
         <v>1</v>
       </c>
-      <c r="M7" s="18"/>
-      <c r="N7" s="11"/>
-      <c r="P7" s="11"/>
+      <c r="M7" s="18">
+        <v>1</v>
+      </c>
+      <c r="N7" s="18"/>
+      <c r="O7" s="11"/>
       <c r="Q7" s="11"/>
       <c r="R7" s="11"/>
       <c r="S7" s="11"/>
@@ -3558,14 +3603,15 @@
       <c r="AT7" s="11"/>
       <c r="AU7" s="11"/>
       <c r="AV7" s="11"/>
-      <c r="AW7" s="2" t="s">
+      <c r="AW7" s="11"/>
+      <c r="AX7" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="AY7" s="2">
+      <c r="AZ7" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>64</v>
       </c>
@@ -3585,45 +3631,48 @@
         <v>0</v>
       </c>
       <c r="G8" s="16">
+        <v>0</v>
+      </c>
+      <c r="H8" s="16">
         <v>1</v>
       </c>
-      <c r="H8" s="16">
+      <c r="I8" s="16">
         <v>0</v>
       </c>
-      <c r="J8" s="16">
+      <c r="K8" s="16">
         <v>0</v>
-      </c>
-      <c r="K8" s="16">
-        <v>1</v>
       </c>
       <c r="L8" s="16">
         <v>1</v>
       </c>
+      <c r="M8" s="16">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="C4:AC4"/>
+    <mergeCell ref="C4:AD4"/>
   </mergeCells>
   <dataValidations count="19">
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showErrorMessage="1" sqref="R7:S1048576">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showErrorMessage="1" sqref="S7:T1048576">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showErrorMessage="1" sqref="AC7:AC1048576 AA7:AA1048576">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showErrorMessage="1" sqref="AD7:AD1048576 AB7:AB1048576">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="list" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V7:V1048576">
+    <dataValidation type="list" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W7:W1048576">
       <formula1>date_choices</formula1>
     </dataValidation>
-    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="O7:O1048576">
+    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="P7:P1048576">
       <formula1>validation_choices</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N7:N1048576">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O7:O1048576">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T7:U1048576 Q7:Q1048576 J7:L1048576 F7:H1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U7:V1048576 R7:R1048576 K7:M1048576 F7:I1048576">
       <formula1>boolean_choices</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P7">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q7">
       <formula1>ouinon</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -3631,31 +3680,31 @@
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AO7 AQ7">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AP7 AR7">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AF7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AG7">
       <formula1>datetype</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AE7">
+    <dataValidation type="list" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AF7">
       <formula1>ouinon</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W7">
-      <formula1>$R$7</formula1>
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X7">
+      <formula1>$S$7</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AK7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AL7">
       <formula1>validation_type</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AJ7">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AK7">
       <formula1>0</formula1>
       <formula2>200</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM7:AN7 AS7:AU7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AN7:AO7 AT7:AV7">
       <formula1>ouinon</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -3665,10 +3714,10 @@
     <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="D7:D1048576">
       <formula1>attribute_groups</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y7:Y1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z7:Z1048576">
       <formula1>metric_types</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z7:Z1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA7:AA1048576">
       <formula1>metric_units</formula1>
     </dataValidation>
   </dataValidations>
@@ -3680,10 +3729,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BB8"/>
+  <dimension ref="A1:BC8"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3693,53 +3742,54 @@
     <col min="4" max="4" width="23.7109375"/>
     <col min="5" max="5" width="16.7109375"/>
     <col min="6" max="6" width="19.7109375" style="16"/>
-    <col min="7" max="7" width="13" style="16"/>
-    <col min="8" max="8" width="25.85546875" style="16"/>
-    <col min="9" max="9" width="25.140625" style="16"/>
-    <col min="10" max="10" width="20"/>
-    <col min="11" max="11" width="23.5703125" style="16"/>
-    <col min="12" max="12" width="23.85546875" style="16"/>
-    <col min="13" max="13" width="20.7109375" style="16"/>
-    <col min="14" max="14" width="13" style="16" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20.42578125"/>
-    <col min="16" max="16" width="19.28515625"/>
-    <col min="17" max="18" width="17.28515625"/>
-    <col min="19" max="19" width="16.5703125"/>
-    <col min="20" max="20" width="19"/>
-    <col min="21" max="22" width="18.7109375"/>
-    <col min="23" max="24" width="13.42578125"/>
-    <col min="25" max="25" width="19.85546875"/>
-    <col min="26" max="26" width="13.42578125"/>
-    <col min="27" max="27" width="18.140625"/>
-    <col min="28" max="28" width="21"/>
-    <col min="29" max="29" width="22"/>
-    <col min="30" max="30" width="23.42578125"/>
-    <col min="31" max="31" width="14.85546875" style="16"/>
-    <col min="32" max="40" width="13.42578125"/>
-    <col min="41" max="41" width="16.85546875"/>
-    <col min="42" max="42" width="19.140625"/>
-    <col min="43" max="43" width="16.28515625"/>
-    <col min="44" max="46" width="13.42578125"/>
-    <col min="47" max="47" width="19.140625"/>
-    <col min="48" max="50" width="18.140625"/>
-    <col min="51" max="51" width="0" style="2" hidden="1"/>
-    <col min="52" max="52" width="0" style="3" hidden="1"/>
-    <col min="53" max="53" width="0" style="2" hidden="1"/>
-    <col min="54" max="54" width="17.140625" style="2"/>
-    <col min="55" max="1025" width="17.140625"/>
+    <col min="7" max="7" width="15.5703125" style="16" customWidth="1"/>
+    <col min="8" max="8" width="13" style="16"/>
+    <col min="9" max="9" width="25.85546875" style="16"/>
+    <col min="10" max="10" width="25.140625" style="16"/>
+    <col min="11" max="11" width="20"/>
+    <col min="12" max="12" width="23.5703125" style="16"/>
+    <col min="13" max="13" width="23.85546875" style="16"/>
+    <col min="14" max="14" width="20.7109375" style="16"/>
+    <col min="15" max="15" width="13" style="16" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.42578125"/>
+    <col min="17" max="17" width="19.28515625"/>
+    <col min="18" max="19" width="17.28515625"/>
+    <col min="20" max="20" width="16.5703125"/>
+    <col min="21" max="21" width="19"/>
+    <col min="22" max="23" width="18.7109375"/>
+    <col min="24" max="25" width="13.42578125"/>
+    <col min="26" max="26" width="19.85546875"/>
+    <col min="27" max="27" width="13.42578125"/>
+    <col min="28" max="28" width="18.140625"/>
+    <col min="29" max="29" width="21"/>
+    <col min="30" max="30" width="22"/>
+    <col min="31" max="31" width="23.42578125"/>
+    <col min="32" max="32" width="14.85546875" style="16"/>
+    <col min="33" max="41" width="13.42578125"/>
+    <col min="42" max="42" width="16.85546875"/>
+    <col min="43" max="43" width="19.140625"/>
+    <col min="44" max="44" width="16.28515625"/>
+    <col min="45" max="47" width="13.42578125"/>
+    <col min="48" max="48" width="19.140625"/>
+    <col min="49" max="51" width="18.140625"/>
+    <col min="52" max="52" width="0" style="2" hidden="1"/>
+    <col min="53" max="53" width="0" style="3" hidden="1"/>
+    <col min="54" max="54" width="0" style="2" hidden="1"/>
+    <col min="55" max="55" width="17.140625" style="2"/>
+    <col min="56" max="1026" width="17.140625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:55" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D1" s="4"/>
       <c r="E1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="AY1"/>
       <c r="AZ1"/>
       <c r="BA1"/>
       <c r="BB1"/>
-    </row>
-    <row r="2" spans="1:54" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BC1"/>
+    </row>
+    <row r="2" spans="1:55" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -3752,12 +3802,12 @@
       <c r="E2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="AY2"/>
       <c r="AZ2"/>
       <c r="BA2"/>
       <c r="BB2"/>
-    </row>
-    <row r="4" spans="1:54" s="19" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BC2"/>
+    </row>
+    <row r="4" spans="1:55" s="19" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="25"/>
       <c r="B4" s="25"/>
       <c r="C4" s="6" t="s">
@@ -3792,11 +3842,12 @@
       <c r="AB4" s="31"/>
       <c r="AC4" s="31"/>
       <c r="AD4" s="31"/>
-      <c r="AE4" s="7" t="s">
+      <c r="AE4" s="31"/>
+      <c r="AF4" s="7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="19" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:55" s="19" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="25" t="s">
         <v>8</v>
       </c>
@@ -3816,82 +3867,85 @@
         <v>12</v>
       </c>
       <c r="G5" s="26" t="s">
+        <v>274</v>
+      </c>
+      <c r="H5" s="26" t="s">
         <v>237</v>
       </c>
-      <c r="H5" s="26" t="s">
+      <c r="I5" s="26" t="s">
         <v>238</v>
       </c>
-      <c r="I5" s="26" t="s">
+      <c r="J5" s="26" t="s">
         <v>239</v>
       </c>
-      <c r="J5" s="26" t="s">
+      <c r="K5" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="K5" s="26" t="s">
+      <c r="L5" s="26" t="s">
         <v>240</v>
       </c>
-      <c r="L5" s="26" t="s">
+      <c r="M5" s="26" t="s">
         <v>241</v>
       </c>
-      <c r="M5" s="26" t="s">
+      <c r="N5" s="26" t="s">
         <v>242</v>
       </c>
-      <c r="N5" s="26" t="s">
+      <c r="O5" s="26" t="s">
         <v>266</v>
       </c>
-      <c r="O5" s="26" t="s">
+      <c r="P5" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="P5" s="26" t="s">
+      <c r="Q5" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="Q5" s="26" t="s">
+      <c r="R5" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="R5" s="26" t="s">
+      <c r="S5" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="S5" s="26" t="s">
+      <c r="T5" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="T5" s="26" t="s">
+      <c r="U5" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="U5" s="26" t="s">
+      <c r="V5" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="V5" s="26" t="s">
+      <c r="W5" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="W5" s="26" t="s">
+      <c r="X5" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="X5" s="26" t="s">
+      <c r="Y5" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="Y5" s="26" t="s">
+      <c r="Z5" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="Z5" s="26" t="s">
+      <c r="AA5" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="AA5" s="26" t="s">
+      <c r="AB5" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="AB5" s="26" t="s">
+      <c r="AC5" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="AC5" s="26" t="s">
+      <c r="AD5" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="AD5" s="26" t="s">
+      <c r="AE5" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="AE5" s="30" t="s">
+      <c r="AF5" s="30" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:54" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:55" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>30</v>
       </c>
@@ -3911,84 +3965,87 @@
         <v>35</v>
       </c>
       <c r="G6" s="17" t="s">
+        <v>273</v>
+      </c>
+      <c r="H6" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="H6" s="17" t="s">
+      <c r="I6" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="I6" s="17" t="s">
+      <c r="J6" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="J6" s="9" t="s">
+      <c r="K6" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="K6" s="17" t="s">
+      <c r="L6" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="L6" s="17" t="s">
+      <c r="M6" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="M6" s="17" t="s">
+      <c r="N6" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="N6" s="17" t="s">
+      <c r="O6" s="17" t="s">
         <v>267</v>
       </c>
-      <c r="O6" s="9" t="s">
+      <c r="P6" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="P6" s="9" t="s">
+      <c r="Q6" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="Q6" s="9" t="s">
+      <c r="R6" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="R6" s="9" t="s">
+      <c r="S6" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="S6" s="9" t="s">
+      <c r="T6" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="T6" s="9" t="s">
+      <c r="U6" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="U6" s="9" t="s">
+      <c r="V6" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="V6" s="9" t="s">
+      <c r="W6" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="W6" s="9" t="s">
+      <c r="X6" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="X6" s="9" t="s">
+      <c r="Y6" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="Y6" s="9" t="s">
+      <c r="Z6" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="Z6" s="9" t="s">
+      <c r="AA6" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="AA6" s="9" t="s">
+      <c r="AB6" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="AB6" s="9" t="s">
+      <c r="AC6" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="AC6" s="9" t="s">
+      <c r="AD6" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="AD6" s="9" t="s">
+      <c r="AE6" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="AE6" s="20"/>
-      <c r="AY6"/>
+      <c r="AF6" s="20"/>
       <c r="AZ6"/>
       <c r="BA6"/>
       <c r="BB6"/>
-    </row>
-    <row r="7" spans="1:54" x14ac:dyDescent="0.2">
+      <c r="BC6"/>
+    </row>
+    <row r="7" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
         <v>59</v>
       </c>
@@ -3997,13 +4054,13 @@
       <c r="G7" s="18"/>
       <c r="H7" s="18"/>
       <c r="I7" s="18"/>
-      <c r="J7" s="11"/>
-      <c r="K7" s="18"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="11"/>
       <c r="L7" s="18"/>
       <c r="M7" s="18"/>
       <c r="N7" s="18"/>
-      <c r="O7" s="11"/>
-      <c r="Q7" s="11"/>
+      <c r="O7" s="18"/>
+      <c r="P7" s="11"/>
       <c r="R7" s="11"/>
       <c r="S7" s="11"/>
       <c r="T7" s="11"/>
@@ -4017,10 +4074,10 @@
       <c r="AB7" s="11"/>
       <c r="AC7" s="11"/>
       <c r="AD7" s="11"/>
-      <c r="AE7" s="18">
+      <c r="AE7" s="11"/>
+      <c r="AF7" s="18">
         <v>1</v>
       </c>
-      <c r="AF7" s="11"/>
       <c r="AG7" s="11"/>
       <c r="AH7" s="11"/>
       <c r="AI7" s="11"/>
@@ -4039,14 +4096,15 @@
       <c r="AV7" s="11"/>
       <c r="AW7" s="11"/>
       <c r="AX7" s="11"/>
-      <c r="AY7" s="2" t="s">
+      <c r="AY7" s="11"/>
+      <c r="AZ7" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="BA7" s="2">
+      <c r="BB7" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>64</v>
       </c>
@@ -4055,40 +4113,40 @@
       </c>
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>
-      <c r="AE8" s="16">
+      <c r="AF8" s="16">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D4:AD4"/>
+    <mergeCell ref="D4:AE4"/>
   </mergeCells>
   <dataValidations count="20">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AO7:AP7 AU7:AW7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AP7:AQ7 AV7:AX7">
       <formula1>ouinon</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AL7">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM7">
       <formula1>0</formula1>
       <formula2>200</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AN7">
       <formula1>validation_type</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X7">
-      <formula1>$S$7</formula1>
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y7">
+      <formula1>$T$7</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AG7">
+    <dataValidation type="list" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AH7">
       <formula1>ouinon</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AH7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AI7">
       <formula1>datetype</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AQ7 AS7">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AR7 AT7">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -4096,29 +4154,29 @@
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q7">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R7">
       <formula1>ouinon</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U7:V1048576 R7:R1048576 B7:B1048576 K7:M1048576 G7:I1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V7:W1048576 S7:S1048576 B7:B1048576 L7:N1048576 G7:J1048576">
       <formula1>boolean_choices</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O7:O1048576">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P7:P1048576">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="P7:P1048576">
+    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="Q7:Q1048576">
       <formula1>validation_choices</formula1>
     </dataValidation>
-    <dataValidation type="list" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W7:W1048576">
+    <dataValidation type="list" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X7:X1048576">
       <formula1>date_choices</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showErrorMessage="1" sqref="AD7:AD1048576 AB7:AB1048576">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showErrorMessage="1" sqref="AE7:AE1048576 AC7:AC1048576">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="AE7:AE1048576">
+    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="AF7:AF1048576">
       <formula1>boolean_choices</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showErrorMessage="1" sqref="S7:T1048576">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showErrorMessage="1" sqref="T7:U1048576">
       <formula1>0</formula1>
     </dataValidation>
     <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="D1:D1048576">
@@ -4127,10 +4185,10 @@
     <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="E1:E1048576">
       <formula1>attribute_groups</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z1:Z1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA1:AA1048576">
       <formula1>metric_types</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA1:AA1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AB1:AB1048576">
       <formula1>metric_units</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Removed properties not used in 1.1
</commit_message>
<xml_diff>
--- a/Resources/fixtures/minimal/init.xlsx
+++ b/Resources/fixtures/minimal/init.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="6990" tabRatio="226" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="6990" tabRatio="226" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="10" r:id="rId1"/>
@@ -23,8 +23,8 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3">attribute_groups!$A$4:$C$4</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1">attributes!$B$6:$AZ$9</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2">'family main'!$C$6:$BB$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1">attributes!$B$6:$AW$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2">'family main'!$C$6:$AY$9</definedName>
     <definedName name="attribute_groups">attribute_groups!$A$4:$A$100</definedName>
     <definedName name="attribute_types">attribute_types!$B$3:$B$14</definedName>
     <definedName name="boolean_choices">choices!$A$1:$A$2</definedName>
@@ -43,20 +43,7 @@
     <author>SMILE</author>
   </authors>
   <commentList>
-    <comment ref="F5" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>The value must be 1 for the identifier, and must be 0 for all other attributes</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="J5" authorId="0">
+    <comment ref="H5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -71,7 +58,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AC5" authorId="0">
+    <comment ref="Z5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -86,7 +73,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AD5" authorId="0">
+    <comment ref="AA5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -110,7 +97,7 @@
     <author>SMILE</author>
   </authors>
   <commentList>
-    <comment ref="AF4" authorId="0">
+    <comment ref="AC4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -123,20 +110,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G5" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>The value must be 1 for the identifier, and must be 0 for all other attributes</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="K5" authorId="0">
+    <comment ref="I5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -151,7 +125,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AD5" authorId="0">
+    <comment ref="AA5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -166,7 +140,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AE5" authorId="0">
+    <comment ref="AB5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -246,7 +220,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="268">
   <si>
     <t>en_US</t>
   </si>
@@ -314,9 +288,6 @@
     <t>Negative allowed</t>
   </si>
   <si>
-    <t>Date type</t>
-  </si>
-  <si>
     <t>Minimum date</t>
   </si>
   <si>
@@ -359,9 +330,6 @@
     <t>unique</t>
   </si>
   <si>
-    <t>searchable</t>
-  </si>
-  <si>
     <t>localizable</t>
   </si>
   <si>
@@ -399,9 +367,6 @@
   </si>
   <si>
     <t>negative_allowed</t>
-  </si>
-  <si>
-    <t>date_type</t>
   </si>
   <si>
     <t>date_min</t>
@@ -1050,9 +1015,6 @@
     <t>Is unique*</t>
   </si>
   <si>
-    <t>Is searchable*</t>
-  </si>
-  <si>
     <t>Is localizable*</t>
   </si>
   <si>
@@ -1173,15 +1135,6 @@
   </si>
   <si>
     <t>Common and unaffected attribute properties</t>
-  </si>
-  <si>
-    <t>Required *</t>
-  </si>
-  <si>
-    <t>required</t>
-  </si>
-  <si>
-    <t>Is required*</t>
   </si>
 </sst>
 </file>
@@ -2041,32 +1994,32 @@
   <sheetData>
     <row r="1" spans="1:2" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A1" s="22" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="21" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B5" s="23" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B6" s="24" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B7" s="24" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B8" s="24" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -2074,7 +2027,7 @@
     </row>
     <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="21" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -2082,127 +2035,127 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B12" s="23" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B15" s="21" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="22" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B22" s="21" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="26" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B26" s="21" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="29" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="31" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B31" s="21" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B34" s="24" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="36" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B36" s="21" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="38" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
     </row>
     <row r="39" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
     </row>
     <row r="41" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B41" s="21" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
     </row>
     <row r="43" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
     </row>
     <row r="45" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B45" s="21" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
     </row>
     <row r="47" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A50" s="29" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B52" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
     </row>
   </sheetData>
@@ -2226,10 +2179,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>208</v>
+      </c>
+      <c r="C1" t="s">
         <v>211</v>
-      </c>
-      <c r="C1" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -2237,18 +2190,18 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>209</v>
+      </c>
+      <c r="C2" t="s">
         <v>212</v>
-      </c>
-      <c r="C2" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
+        <v>210</v>
+      </c>
+      <c r="C3" t="s">
         <v>213</v>
-      </c>
-      <c r="C3" t="s">
-        <v>216</v>
       </c>
     </row>
   </sheetData>
@@ -2273,114 +2226,114 @@
   <sheetData>
     <row r="1" spans="1:2" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B5" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B6" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B7" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B8" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B9" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B10" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B11" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B12" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B13" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B14" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -2410,90 +2363,90 @@
   <sheetData>
     <row r="1" spans="1:2" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B5" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B6" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B7" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B8" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B9" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B10" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B11" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -2523,714 +2476,714 @@
   <sheetData>
     <row r="1" spans="1:1024" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B1" s="9"/>
       <c r="AMJ1"/>
     </row>
     <row r="2" spans="1:1024" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="AMJ2"/>
     </row>
     <row r="3" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B3" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B4" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B5" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="6" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B6" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="7" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B7" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="8" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B8" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="9" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B9" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="10" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B10" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="11" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B11" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="12" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B12" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="13" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B13" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="14" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B14" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="15" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B15" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="16" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B16" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B17" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B18" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B19" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B20" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B21" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B22" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B23" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B24" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B25" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B26" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B27" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B28" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B29" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B30" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B31" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B32" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B33" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B34" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B35" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B36" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B37" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B38" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B39" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B40" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B41" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B42" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B43" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B44" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B45" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B46" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B47" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B48" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B49" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B50" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B51" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B52" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B53" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B54" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B55" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B56" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B57" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B58" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B59" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B60" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B61" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B62" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B63" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B64" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B65" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B66" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B67" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B68" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B69" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B70" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B71" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B72" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B73" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B74" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B75" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B76" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B77" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B78" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B79" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B80" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B81" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B82" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B83" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B84" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B85" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B86" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B87" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B88" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B89" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
   </sheetData>
@@ -3245,10 +3198,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BA8"/>
+  <dimension ref="A1:AX8"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="T13" sqref="T13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3258,56 +3211,53 @@
     <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.85546875" style="16" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" style="16" customWidth="1"/>
-    <col min="7" max="7" width="10.140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.85546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.7109375" style="16" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23.42578125" style="16" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.5703125" style="16" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.28515625" style="16" customWidth="1"/>
-    <col min="15" max="15" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="17" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="14" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="19" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="21" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="9.140625" style="2"/>
-    <col min="51" max="51" width="9.140625" style="3"/>
-    <col min="52" max="53" width="9.140625" style="2"/>
+    <col min="6" max="6" width="10.140625" style="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" style="16" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" style="16" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.42578125" style="16" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.5703125" style="16" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.28515625" style="16" customWidth="1"/>
+    <col min="13" max="13" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="19" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="21" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="9.140625" style="2"/>
+    <col min="48" max="48" width="9.140625" style="3"/>
+    <col min="49" max="50" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:50" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="24" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
+      <c r="AU1"/>
+      <c r="AV1"/>
+      <c r="AW1"/>
       <c r="AX1"/>
-      <c r="AY1"/>
-      <c r="AZ1"/>
-      <c r="BA1"/>
-    </row>
-    <row r="2" spans="1:53" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:50" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4"/>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
+      <c r="AU2"/>
+      <c r="AV2"/>
+      <c r="AW2"/>
       <c r="AX2"/>
-      <c r="AY2"/>
-      <c r="AZ2"/>
-      <c r="BA2"/>
-    </row>
-    <row r="4" spans="1:53" s="19" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:50" s="19" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="25"/>
       <c r="B4" s="6" t="s">
         <v>5</v>
@@ -3339,11 +3289,8 @@
       <c r="Y4" s="31"/>
       <c r="Z4" s="31"/>
       <c r="AA4" s="31"/>
-      <c r="AB4" s="31"/>
-      <c r="AC4" s="31"/>
-      <c r="AD4" s="31"/>
-    </row>
-    <row r="5" spans="1:53" s="19" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:50" s="19" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="25" t="s">
         <v>8</v>
       </c>
@@ -3360,123 +3307,114 @@
         <v>12</v>
       </c>
       <c r="F5" s="26" t="s">
-        <v>272</v>
+        <v>234</v>
       </c>
       <c r="G5" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="H5" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="I5" s="26" t="s">
+        <v>236</v>
+      </c>
+      <c r="J5" s="26" t="s">
         <v>237</v>
       </c>
-      <c r="H5" s="26" t="s">
+      <c r="K5" s="26" t="s">
         <v>238</v>
       </c>
-      <c r="I5" s="26" t="s">
-        <v>239</v>
-      </c>
-      <c r="J5" s="26" t="s">
-        <v>13</v>
-      </c>
-      <c r="K5" s="26" t="s">
-        <v>240</v>
-      </c>
       <c r="L5" s="26" t="s">
-        <v>241</v>
+        <v>262</v>
       </c>
       <c r="M5" s="26" t="s">
-        <v>242</v>
+        <v>14</v>
       </c>
       <c r="N5" s="26" t="s">
-        <v>266</v>
+        <v>15</v>
       </c>
       <c r="O5" s="26" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="P5" s="26" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="Q5" s="26" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="R5" s="26" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="S5" s="26" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="T5" s="26" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="U5" s="26" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="V5" s="26" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="W5" s="26" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="X5" s="26" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="Y5" s="26" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="Z5" s="26" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="AA5" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="AB5" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC5" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="AD5" s="26" t="s">
+    </row>
+    <row r="6" spans="1:50" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="6" spans="1:53" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
-        <v>30</v>
-      </c>
       <c r="B6" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="D6" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="E6" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="E6" s="17" t="s">
+      <c r="F6" s="17" t="s">
         <v>35</v>
-      </c>
-      <c r="F6" s="17" t="s">
-        <v>273</v>
       </c>
       <c r="G6" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="H6" s="17" t="s">
+      <c r="H6" s="9" t="s">
         <v>37</v>
       </c>
       <c r="I6" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="J6" s="9" t="s">
+      <c r="J6" s="17" t="s">
         <v>39</v>
       </c>
       <c r="K6" s="17" t="s">
         <v>40</v>
       </c>
       <c r="L6" s="17" t="s">
+        <v>263</v>
+      </c>
+      <c r="M6" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="M6" s="17" t="s">
+      <c r="N6" s="9" t="s">
         <v>42</v>
-      </c>
-      <c r="N6" s="17" t="s">
-        <v>267</v>
       </c>
       <c r="O6" s="9" t="s">
         <v>43</v>
@@ -3517,32 +3455,23 @@
       <c r="AA6" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="AB6" s="9" t="s">
+      <c r="AU6"/>
+      <c r="AV6"/>
+      <c r="AW6"/>
+      <c r="AX6"/>
+    </row>
+    <row r="7" spans="1:50" x14ac:dyDescent="0.2">
+      <c r="A7" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="AC6" s="9" t="s">
+      <c r="B7" t="s">
         <v>57</v>
       </c>
-      <c r="AD6" s="9" t="s">
+      <c r="C7" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="AX6"/>
-      <c r="AY6"/>
-      <c r="AZ6"/>
-      <c r="BA6"/>
-    </row>
-    <row r="7" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A7" s="10" t="s">
+      <c r="D7" s="10" t="s">
         <v>59</v>
-      </c>
-      <c r="B7" t="s">
-        <v>60</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>62</v>
       </c>
       <c r="E7" s="16">
         <v>1</v>
@@ -3551,26 +3480,22 @@
         <v>1</v>
       </c>
       <c r="G7" s="18">
-        <v>1</v>
-      </c>
-      <c r="H7" s="18">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="H7" s="11"/>
       <c r="I7" s="18">
         <v>0</v>
       </c>
-      <c r="J7" s="11"/>
+      <c r="J7" s="18">
+        <v>1</v>
+      </c>
       <c r="K7" s="18">
-        <v>0</v>
-      </c>
-      <c r="L7" s="18">
         <v>1</v>
       </c>
-      <c r="M7" s="18">
-        <v>1</v>
-      </c>
-      <c r="N7" s="18"/>
+      <c r="L7" s="18"/>
+      <c r="M7" s="11"/>
       <c r="O7" s="11"/>
+      <c r="P7" s="11"/>
       <c r="Q7" s="11"/>
       <c r="R7" s="11"/>
       <c r="S7" s="11"/>
@@ -3601,28 +3526,25 @@
       <c r="AR7" s="11"/>
       <c r="AS7" s="11"/>
       <c r="AT7" s="11"/>
-      <c r="AU7" s="11"/>
-      <c r="AV7" s="11"/>
-      <c r="AW7" s="11"/>
-      <c r="AX7" s="2" t="s">
+      <c r="AU7" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AW7" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:50" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C8" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="AZ7" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>64</v>
-      </c>
-      <c r="B8" t="s">
-        <v>65</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>66</v>
-      </c>
       <c r="D8" s="10" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E8" s="16">
         <v>2</v>
@@ -3633,46 +3555,37 @@
       <c r="G8" s="16">
         <v>0</v>
       </c>
-      <c r="H8" s="16">
-        <v>1</v>
-      </c>
       <c r="I8" s="16">
         <v>0</v>
       </c>
+      <c r="J8" s="16">
+        <v>1</v>
+      </c>
       <c r="K8" s="16">
-        <v>0</v>
-      </c>
-      <c r="L8" s="16">
-        <v>1</v>
-      </c>
-      <c r="M8" s="16">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="C4:AD4"/>
+    <mergeCell ref="C4:AA4"/>
   </mergeCells>
-  <dataValidations count="19">
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showErrorMessage="1" sqref="S7:T1048576">
+  <dataValidations count="18">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showErrorMessage="1" sqref="Q7:R1048576">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showErrorMessage="1" sqref="AD7:AD1048576 AB7:AB1048576">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showErrorMessage="1" sqref="AA7:AA1048576 Y7:Y1048576">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="list" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W7:W1048576">
-      <formula1>date_choices</formula1>
-    </dataValidation>
-    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="P7:P1048576">
+    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="N7:N1048576">
       <formula1>validation_choices</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O7:O1048576">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M7:M1048576">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U7:V1048576 R7:R1048576 K7:M1048576 F7:I1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S7:T1048576 P7:P1048576 I7:K1048576 F7:G1048576">
       <formula1>boolean_choices</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q7">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O7">
       <formula1>ouinon</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -3680,31 +3593,31 @@
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AP7 AR7">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM7 AO7">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AG7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AD7">
       <formula1>datetype</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AF7">
+    <dataValidation type="list" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AC7">
       <formula1>ouinon</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X7">
-      <formula1>$S$7</formula1>
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U7">
+      <formula1>$Q$7</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AL7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AI7">
       <formula1>validation_type</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AK7">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AH7">
       <formula1>0</formula1>
       <formula2>200</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AN7:AO7 AT7:AV7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AK7:AL7 AQ7:AS7">
       <formula1>ouinon</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -3714,10 +3627,10 @@
     <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="D7:D1048576">
       <formula1>attribute_groups</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z7:Z1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W7:W1048576">
       <formula1>metric_types</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA7:AA1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X7:X1048576">
       <formula1>metric_units</formula1>
     </dataValidation>
   </dataValidations>
@@ -3729,10 +3642,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BC8"/>
+  <dimension ref="A1:AZ8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView topLeftCell="T1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="V1" sqref="V1:V1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3742,54 +3655,52 @@
     <col min="4" max="4" width="23.7109375"/>
     <col min="5" max="5" width="16.7109375"/>
     <col min="6" max="6" width="19.7109375" style="16"/>
-    <col min="7" max="7" width="15.5703125" style="16" customWidth="1"/>
-    <col min="8" max="8" width="13" style="16"/>
-    <col min="9" max="9" width="25.85546875" style="16"/>
-    <col min="10" max="10" width="25.140625" style="16"/>
-    <col min="11" max="11" width="20"/>
-    <col min="12" max="12" width="23.5703125" style="16"/>
-    <col min="13" max="13" width="23.85546875" style="16"/>
-    <col min="14" max="14" width="20.7109375" style="16"/>
-    <col min="15" max="15" width="13" style="16" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20.42578125"/>
-    <col min="17" max="17" width="19.28515625"/>
-    <col min="18" max="19" width="17.28515625"/>
-    <col min="20" max="20" width="16.5703125"/>
-    <col min="21" max="21" width="19"/>
-    <col min="22" max="23" width="18.7109375"/>
-    <col min="24" max="25" width="13.42578125"/>
-    <col min="26" max="26" width="19.85546875"/>
-    <col min="27" max="27" width="13.42578125"/>
-    <col min="28" max="28" width="18.140625"/>
-    <col min="29" max="29" width="21"/>
-    <col min="30" max="30" width="22"/>
-    <col min="31" max="31" width="23.42578125"/>
-    <col min="32" max="32" width="14.85546875" style="16"/>
-    <col min="33" max="41" width="13.42578125"/>
-    <col min="42" max="42" width="16.85546875"/>
-    <col min="43" max="43" width="19.140625"/>
-    <col min="44" max="44" width="16.28515625"/>
-    <col min="45" max="47" width="13.42578125"/>
-    <col min="48" max="48" width="19.140625"/>
-    <col min="49" max="51" width="18.140625"/>
-    <col min="52" max="52" width="0" style="2" hidden="1"/>
-    <col min="53" max="53" width="0" style="3" hidden="1"/>
-    <col min="54" max="54" width="0" style="2" hidden="1"/>
-    <col min="55" max="55" width="17.140625" style="2"/>
-    <col min="56" max="1026" width="17.140625"/>
+    <col min="7" max="7" width="13" style="16"/>
+    <col min="8" max="8" width="25.140625" style="16"/>
+    <col min="9" max="9" width="20"/>
+    <col min="10" max="10" width="23.5703125" style="16"/>
+    <col min="11" max="11" width="23.85546875" style="16"/>
+    <col min="12" max="12" width="20.7109375" style="16"/>
+    <col min="13" max="13" width="13" style="16" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.42578125"/>
+    <col min="15" max="15" width="19.28515625"/>
+    <col min="16" max="17" width="17.28515625"/>
+    <col min="18" max="18" width="16.5703125"/>
+    <col min="19" max="19" width="19"/>
+    <col min="20" max="21" width="18.7109375"/>
+    <col min="22" max="22" width="13.42578125"/>
+    <col min="23" max="23" width="19.85546875"/>
+    <col min="24" max="24" width="13.42578125"/>
+    <col min="25" max="25" width="18.140625"/>
+    <col min="26" max="26" width="21"/>
+    <col min="27" max="27" width="22"/>
+    <col min="28" max="28" width="23.42578125"/>
+    <col min="29" max="29" width="14.85546875" style="16"/>
+    <col min="30" max="38" width="13.42578125"/>
+    <col min="39" max="39" width="16.85546875"/>
+    <col min="40" max="40" width="19.140625"/>
+    <col min="41" max="41" width="16.28515625"/>
+    <col min="42" max="44" width="13.42578125"/>
+    <col min="45" max="45" width="19.140625"/>
+    <col min="46" max="48" width="18.140625"/>
+    <col min="49" max="49" width="0" style="2" hidden="1"/>
+    <col min="50" max="50" width="0" style="3" hidden="1"/>
+    <col min="51" max="51" width="0" style="2" hidden="1"/>
+    <col min="52" max="52" width="17.140625" style="2"/>
+    <col min="53" max="1023" width="17.140625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:55" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:52" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D1" s="4"/>
       <c r="E1" s="4" t="s">
         <v>0</v>
       </c>
+      <c r="AW1"/>
+      <c r="AX1"/>
+      <c r="AY1"/>
       <c r="AZ1"/>
-      <c r="BA1"/>
-      <c r="BB1"/>
-      <c r="BC1"/>
-    </row>
-    <row r="2" spans="1:55" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:52" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -3802,12 +3713,12 @@
       <c r="E2" s="4" t="s">
         <v>4</v>
       </c>
+      <c r="AW2"/>
+      <c r="AX2"/>
+      <c r="AY2"/>
       <c r="AZ2"/>
-      <c r="BA2"/>
-      <c r="BB2"/>
-      <c r="BC2"/>
-    </row>
-    <row r="4" spans="1:55" s="19" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:52" s="19" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="25"/>
       <c r="B4" s="25"/>
       <c r="C4" s="6" t="s">
@@ -3840,14 +3751,11 @@
       <c r="Z4" s="31"/>
       <c r="AA4" s="31"/>
       <c r="AB4" s="31"/>
-      <c r="AC4" s="31"/>
-      <c r="AD4" s="31"/>
-      <c r="AE4" s="31"/>
-      <c r="AF4" s="7" t="s">
+      <c r="AC4" s="7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:55" s="19" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:52" s="19" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="25" t="s">
         <v>8</v>
       </c>
@@ -3867,129 +3775,120 @@
         <v>12</v>
       </c>
       <c r="G5" s="26" t="s">
-        <v>274</v>
+        <v>234</v>
       </c>
       <c r="H5" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="I5" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="J5" s="26" t="s">
+        <v>236</v>
+      </c>
+      <c r="K5" s="26" t="s">
         <v>237</v>
       </c>
-      <c r="I5" s="26" t="s">
+      <c r="L5" s="26" t="s">
         <v>238</v>
       </c>
-      <c r="J5" s="26" t="s">
-        <v>239</v>
-      </c>
-      <c r="K5" s="26" t="s">
-        <v>13</v>
-      </c>
-      <c r="L5" s="26" t="s">
-        <v>240</v>
-      </c>
       <c r="M5" s="26" t="s">
-        <v>241</v>
+        <v>262</v>
       </c>
       <c r="N5" s="26" t="s">
-        <v>242</v>
+        <v>14</v>
       </c>
       <c r="O5" s="26" t="s">
-        <v>266</v>
+        <v>15</v>
       </c>
       <c r="P5" s="26" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="Q5" s="26" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="R5" s="26" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="S5" s="26" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="T5" s="26" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="U5" s="26" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="V5" s="26" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="W5" s="26" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="X5" s="26" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="Y5" s="26" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="Z5" s="26" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="AA5" s="26" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="AB5" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="AC5" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="AD5" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="AE5" s="26" t="s">
+      <c r="AC5" s="30" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:52" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="AF5" s="30" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:55" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
+      <c r="B6" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="C6" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="D6" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="E6" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="F6" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="F6" s="17" t="s">
+      <c r="G6" s="17" t="s">
         <v>35</v>
-      </c>
-      <c r="G6" s="17" t="s">
-        <v>273</v>
       </c>
       <c r="H6" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="I6" s="17" t="s">
+      <c r="I6" s="9" t="s">
         <v>37</v>
       </c>
       <c r="J6" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="K6" s="9" t="s">
+      <c r="K6" s="17" t="s">
         <v>39</v>
       </c>
       <c r="L6" s="17" t="s">
         <v>40</v>
       </c>
       <c r="M6" s="17" t="s">
+        <v>263</v>
+      </c>
+      <c r="N6" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="N6" s="17" t="s">
+      <c r="O6" s="9" t="s">
         <v>42</v>
-      </c>
-      <c r="O6" s="17" t="s">
-        <v>267</v>
       </c>
       <c r="P6" s="9" t="s">
         <v>43</v>
@@ -4030,37 +3929,28 @@
       <c r="AB6" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="AC6" s="9" t="s">
+      <c r="AC6" s="20"/>
+      <c r="AW6"/>
+      <c r="AX6"/>
+      <c r="AY6"/>
+      <c r="AZ6"/>
+    </row>
+    <row r="7" spans="1:52" x14ac:dyDescent="0.2">
+      <c r="A7" s="10" t="s">
         <v>56</v>
-      </c>
-      <c r="AD6" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="AE6" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="AF6" s="20"/>
-      <c r="AZ6"/>
-      <c r="BA6"/>
-      <c r="BB6"/>
-      <c r="BC6"/>
-    </row>
-    <row r="7" spans="1:55" x14ac:dyDescent="0.2">
-      <c r="A7" s="10" t="s">
-        <v>59</v>
       </c>
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
       <c r="G7" s="18"/>
       <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
+      <c r="I7" s="11"/>
       <c r="J7" s="18"/>
-      <c r="K7" s="11"/>
+      <c r="K7" s="18"/>
       <c r="L7" s="18"/>
       <c r="M7" s="18"/>
-      <c r="N7" s="18"/>
-      <c r="O7" s="18"/>
+      <c r="N7" s="11"/>
       <c r="P7" s="11"/>
+      <c r="Q7" s="11"/>
       <c r="R7" s="11"/>
       <c r="S7" s="11"/>
       <c r="T7" s="11"/>
@@ -4072,12 +3962,12 @@
       <c r="Z7" s="11"/>
       <c r="AA7" s="11"/>
       <c r="AB7" s="11"/>
-      <c r="AC7" s="11"/>
+      <c r="AC7" s="18">
+        <v>1</v>
+      </c>
       <c r="AD7" s="11"/>
       <c r="AE7" s="11"/>
-      <c r="AF7" s="18">
-        <v>1</v>
-      </c>
+      <c r="AF7" s="11"/>
       <c r="AG7" s="11"/>
       <c r="AH7" s="11"/>
       <c r="AI7" s="11"/>
@@ -4094,59 +3984,56 @@
       <c r="AT7" s="11"/>
       <c r="AU7" s="11"/>
       <c r="AV7" s="11"/>
-      <c r="AW7" s="11"/>
-      <c r="AX7" s="11"/>
-      <c r="AY7" s="11"/>
-      <c r="AZ7" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="BB7" s="2">
+      <c r="AW7" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AY7" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>
-      <c r="AF8" s="16">
+      <c r="AC8" s="16">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D4:AE4"/>
+    <mergeCell ref="D4:AB4"/>
   </mergeCells>
-  <dataValidations count="20">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AP7:AQ7 AV7:AX7">
+  <dataValidations count="19">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM7:AN7 AS7:AU7">
       <formula1>ouinon</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM7">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AJ7">
       <formula1>0</formula1>
       <formula2>200</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AN7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AK7">
       <formula1>validation_type</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y7">
-      <formula1>$T$7</formula1>
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V7">
+      <formula1>$R$7</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AH7">
+    <dataValidation type="list" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AE7">
       <formula1>ouinon</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AI7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AF7">
       <formula1>datetype</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AR7 AT7">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AO7 AQ7">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -4154,29 +4041,26 @@
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R7">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P7">
       <formula1>ouinon</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V7:W1048576 S7:S1048576 B7:B1048576 L7:N1048576 G7:J1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T7:U1048576 Q7:Q1048576 B7:B1048576 J7:L1048576 G7:H1048576">
       <formula1>boolean_choices</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P7:P1048576">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N7:N1048576">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="Q7:Q1048576">
+    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="O7:O1048576">
       <formula1>validation_choices</formula1>
     </dataValidation>
-    <dataValidation type="list" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X7:X1048576">
-      <formula1>date_choices</formula1>
-    </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showErrorMessage="1" sqref="AE7:AE1048576 AC7:AC1048576">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showErrorMessage="1" sqref="AB7:AB1048576 Z7:Z1048576">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="AF7:AF1048576">
+    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="AC7:AC1048576">
       <formula1>boolean_choices</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showErrorMessage="1" sqref="T7:U1048576">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showErrorMessage="1" sqref="R7:S1048576">
       <formula1>0</formula1>
     </dataValidation>
     <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="D1:D1048576">
@@ -4185,10 +4069,10 @@
     <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="E1:E1048576">
       <formula1>attribute_groups</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA1:AA1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X1:X1048576">
       <formula1>metric_types</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AB1:AB1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y1:Y1048576">
       <formula1>metric_units</formula1>
     </dataValidation>
   </dataValidations>
@@ -4216,7 +4100,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="32" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B1" s="32"/>
       <c r="C1" s="13" t="s">
@@ -4225,10 +4109,10 @@
     </row>
     <row r="2" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C2" s="14" t="s">
         <v>0</v>
@@ -4236,24 +4120,24 @@
     </row>
     <row r="3" spans="1:3" ht="24.4" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B4" s="11">
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -4283,7 +4167,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="32" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B1" s="32"/>
       <c r="C1" s="32"/>
@@ -4296,10 +4180,10 @@
         <v>8</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D2" s="14" t="s">
         <v>0</v>
@@ -4307,16 +4191,16 @@
     </row>
     <row r="3" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -4355,7 +4239,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="32" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B1" s="32"/>
       <c r="C1" s="32"/>
@@ -4364,36 +4248,36 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="D2" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="E2" s="9" t="s">
         <v>78</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4407,7 +4291,7 @@
         <v>0</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E4" s="11" t="s">
         <v>2</v>
@@ -4447,7 +4331,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="32" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B1" s="32"/>
       <c r="C1" s="13" t="s">
@@ -4456,10 +4340,10 @@
     </row>
     <row r="2" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C2" s="14" t="s">
         <v>0</v>
@@ -4467,13 +4351,13 @@
     </row>
     <row r="3" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4481,7 +4365,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -4516,29 +4400,29 @@
   <sheetData>
     <row r="1" spans="1:2" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="32" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="B1" s="32"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
     </row>
     <row r="3" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -4546,7 +4430,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -4580,7 +4464,7 @@
   <sheetData>
     <row r="1" spans="1:2" s="28" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>5</v>
@@ -4588,7 +4472,7 @@
     </row>
     <row r="2" spans="1:2" s="28" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="26" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="B2" s="13" t="s">
         <v>0</v>
@@ -4596,42 +4480,42 @@
     </row>
     <row r="3" spans="1:2" s="28" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="B4" s="27" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="B5" s="28" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="B6" s="28" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="B7" s="28" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Upgraded fixtures to 1.3 version of Akeneo PIM CE
</commit_message>
<xml_diff>
--- a/Resources/fixtures/minimal/init.xlsx
+++ b/Resources/fixtures/minimal/init.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="6990" tabRatio="226" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="6570" tabRatio="226"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="10" r:id="rId1"/>
@@ -23,8 +23,8 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3">attribute_groups!$A$4:$C$4</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1">attributes!$B$6:$AW$9</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2">'family main'!$C$6:$AY$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1">attributes!$B$6:$AU$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2">'family main'!$C$6:$AW$9</definedName>
     <definedName name="attribute_groups">attribute_groups!$A$4:$A$100</definedName>
     <definedName name="attribute_types">attribute_types!$B$3:$B$14</definedName>
     <definedName name="boolean_choices">choices!$A$1:$A$2</definedName>
@@ -58,7 +58,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Z5" authorId="0">
+    <comment ref="X5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -73,7 +73,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AA5" authorId="0">
+    <comment ref="Y5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -97,7 +97,7 @@
     <author>SMILE</author>
   </authors>
   <commentList>
-    <comment ref="AC4" authorId="0">
+    <comment ref="AA4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -125,7 +125,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AA5" authorId="0">
+    <comment ref="Y5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -140,7 +140,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AB5" authorId="0">
+    <comment ref="Z5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -159,29 +159,6 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>SMILE</author>
-  </authors>
-  <commentList>
-    <comment ref="C2" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Each attribute should have only one default option</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>SMILE</author>
@@ -220,7 +197,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="263">
   <si>
     <t>en_US</t>
   </si>
@@ -339,9 +316,6 @@
     <t>scopable</t>
   </si>
   <si>
-    <t>useable_as_grid_column</t>
-  </si>
-  <si>
     <t>useable_as_grid_filter</t>
   </si>
   <si>
@@ -354,9 +328,6 @@
     <t>validation_regexp</t>
   </si>
   <si>
-    <t>wisiwig_enabled</t>
-  </si>
-  <si>
     <t>number_min</t>
   </si>
   <si>
@@ -432,13 +403,7 @@
     <t>Option code</t>
   </si>
   <si>
-    <t>Is default</t>
-  </si>
-  <si>
     <t>attribute</t>
-  </si>
-  <si>
-    <t>default</t>
   </si>
   <si>
     <t>Channel properties</t>
@@ -1021,9 +986,6 @@
     <t>Is scopable*</t>
   </si>
   <si>
-    <t>Useable as grid column*</t>
-  </si>
-  <si>
     <t>Useable as grid filter*</t>
   </si>
   <si>
@@ -1105,12 +1067,6 @@
       </rPr>
       <t>save this file with another extension than xlsx</t>
     </r>
-  </si>
-  <si>
-    <t>Default value</t>
-  </si>
-  <si>
-    <t>default_value</t>
   </si>
   <si>
     <t>Attributes tab</t>
@@ -1135,6 +1091,12 @@
   </si>
   <si>
     <t>Common and unaffected attribute properties</t>
+  </si>
+  <si>
+    <t>wysiwyg_enabled</t>
+  </si>
+  <si>
+    <t>available_locales</t>
   </si>
 </sst>
 </file>
@@ -1431,7 +1393,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>847725</xdr:colOff>
       <xdr:row>59</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
@@ -1474,7 +1436,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>847725</xdr:colOff>
       <xdr:row>59</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
@@ -1983,9 +1945,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B53"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:XFD17"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1994,32 +1954,32 @@
   <sheetData>
     <row r="1" spans="1:2" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A1" s="22" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="21" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B5" s="23" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B6" s="24" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B7" s="24" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B8" s="24" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -2027,7 +1987,7 @@
     </row>
     <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="21" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -2035,127 +1995,127 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B12" s="23" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B15" s="21" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
     </row>
     <row r="22" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B22" s="21" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
     </row>
     <row r="26" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B26" s="21" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
     </row>
     <row r="29" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="31" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B31" s="21" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B34" s="24" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
     </row>
     <row r="36" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B36" s="21" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
     </row>
     <row r="38" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
     </row>
     <row r="39" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
     </row>
     <row r="41" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B41" s="21" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
     </row>
     <row r="43" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
     </row>
     <row r="45" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B45" s="21" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
     </row>
     <row r="47" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A50" s="29" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B52" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
     </row>
   </sheetData>
@@ -2179,10 +2139,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="C1" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -2190,18 +2150,18 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="C2" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="C3" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
   </sheetData>
@@ -2226,10 +2186,10 @@
   <sheetData>
     <row r="1" spans="1:2" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -2237,103 +2197,103 @@
         <v>29</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B5" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B6" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B7" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B8" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B9" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B10" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B11" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B12" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B13" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B14" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -2363,10 +2323,10 @@
   <sheetData>
     <row r="1" spans="1:2" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -2374,79 +2334,79 @@
         <v>29</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B3" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B4" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B5" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B6" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B7" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B8" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B9" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B10" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B11" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -2476,7 +2436,7 @@
   <sheetData>
     <row r="1" spans="1:1024" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B1" s="9"/>
       <c r="AMJ1"/>
@@ -2486,704 +2446,704 @@
         <v>32</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="AMJ2"/>
     </row>
     <row r="3" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B3" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B4" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B5" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B6" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="7" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B7" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="8" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B8" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="9" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B9" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="10" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B10" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="11" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B11" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="12" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B12" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="13" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B13" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="14" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B14" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="15" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B15" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="16" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B16" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B17" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B18" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B19" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B20" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B21" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B22" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B23" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B24" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B25" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B26" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B27" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B28" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B29" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B30" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B31" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B32" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B33" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B34" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B35" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B36" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B37" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B38" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B39" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B40" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B41" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B42" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B43" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B44" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B45" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B46" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B47" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B48" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B49" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B50" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B51" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B52" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B53" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B54" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B55" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B56" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B57" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B58" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B59" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B60" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B61" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B62" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B63" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B64" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B65" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B66" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B67" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B68" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B69" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B70" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B71" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B72" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B73" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B74" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B75" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B76" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B77" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B78" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B79" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B80" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B81" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B82" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B83" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B85" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B86" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B87" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B88" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B89" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
     </row>
   </sheetData>
@@ -3198,11 +3158,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AX8"/>
+  <dimension ref="A1:AV8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="T13" sqref="T13"/>
-    </sheetView>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3215,49 +3173,47 @@
     <col min="7" max="7" width="13.7109375" style="16" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.42578125" style="16" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.5703125" style="16" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.28515625" style="16" customWidth="1"/>
-    <col min="13" max="13" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="17" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="19" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="21" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="9.140625" style="2"/>
-    <col min="48" max="48" width="9.140625" style="3"/>
-    <col min="49" max="50" width="9.140625" style="2"/>
+    <col min="10" max="10" width="20.5703125" style="16" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="19" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="21" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="9.140625" style="2"/>
+    <col min="46" max="46" width="9.140625" style="3"/>
+    <col min="47" max="48" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:48" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="24" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
+      <c r="AS1"/>
+      <c r="AT1"/>
       <c r="AU1"/>
       <c r="AV1"/>
-      <c r="AW1"/>
-      <c r="AX1"/>
-    </row>
-    <row r="2" spans="1:50" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:48" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4"/>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
+      <c r="AS2"/>
+      <c r="AT2"/>
       <c r="AU2"/>
       <c r="AV2"/>
-      <c r="AW2"/>
-      <c r="AX2"/>
-    </row>
-    <row r="4" spans="1:50" s="19" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:48" s="19" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="25"/>
       <c r="B4" s="6" t="s">
         <v>5</v>
@@ -3287,10 +3243,8 @@
       <c r="W4" s="31"/>
       <c r="X4" s="31"/>
       <c r="Y4" s="31"/>
-      <c r="Z4" s="31"/>
-      <c r="AA4" s="31"/>
-    </row>
-    <row r="5" spans="1:50" s="19" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:48" s="19" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="25" t="s">
         <v>8</v>
       </c>
@@ -3307,73 +3261,67 @@
         <v>12</v>
       </c>
       <c r="F5" s="26" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="G5" s="26" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="H5" s="26" t="s">
         <v>13</v>
       </c>
       <c r="I5" s="26" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="J5" s="26" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="K5" s="26" t="s">
-        <v>238</v>
+        <v>14</v>
       </c>
       <c r="L5" s="26" t="s">
-        <v>262</v>
+        <v>15</v>
       </c>
       <c r="M5" s="26" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="N5" s="26" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="O5" s="26" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="P5" s="26" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="Q5" s="26" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="R5" s="26" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="S5" s="26" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="T5" s="26" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="U5" s="26" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="V5" s="26" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="W5" s="26" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="X5" s="26" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="Y5" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="Z5" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="AA5" s="26" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:50" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:48" ht="38.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>29</v>
       </c>
@@ -3396,7 +3344,7 @@
         <v>36</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>37</v>
+        <v>262</v>
       </c>
       <c r="I6" s="17" t="s">
         <v>38</v>
@@ -3404,17 +3352,17 @@
       <c r="J6" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="K6" s="17" t="s">
+      <c r="K6" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="L6" s="17" t="s">
-        <v>263</v>
+      <c r="L6" s="9" t="s">
+        <v>41</v>
       </c>
       <c r="M6" s="9" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="N6" s="9" t="s">
-        <v>42</v>
+        <v>261</v>
       </c>
       <c r="O6" s="9" t="s">
         <v>43</v>
@@ -3449,29 +3397,23 @@
       <c r="Y6" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="Z6" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="AA6" s="9" t="s">
-        <v>55</v>
-      </c>
+      <c r="AS6"/>
+      <c r="AT6"/>
       <c r="AU6"/>
       <c r="AV6"/>
-      <c r="AW6"/>
-      <c r="AX6"/>
-    </row>
-    <row r="7" spans="1:50" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="B7" t="s">
+      <c r="D7" s="10" t="s">
         <v>57</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>59</v>
       </c>
       <c r="E7" s="16">
         <v>1</v>
@@ -3489,11 +3431,9 @@
       <c r="J7" s="18">
         <v>1</v>
       </c>
-      <c r="K7" s="18">
-        <v>1</v>
-      </c>
-      <c r="L7" s="18"/>
+      <c r="K7" s="11"/>
       <c r="M7" s="11"/>
+      <c r="N7" s="11"/>
       <c r="O7" s="11"/>
       <c r="P7" s="11"/>
       <c r="Q7" s="11"/>
@@ -3524,27 +3464,19 @@
       <c r="AP7" s="11"/>
       <c r="AQ7" s="11"/>
       <c r="AR7" s="11"/>
-      <c r="AS7" s="11"/>
-      <c r="AT7" s="11"/>
-      <c r="AU7" s="2" t="s">
+    </row>
+    <row r="8" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B8" t="s">
         <v>60</v>
       </c>
-      <c r="AW7" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:50" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="C8" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="B8" t="s">
-        <v>62</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>63</v>
-      </c>
       <c r="D8" s="10" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E8" s="16">
         <v>2</v>
@@ -3561,31 +3493,28 @@
       <c r="J8" s="16">
         <v>1</v>
       </c>
-      <c r="K8" s="16">
-        <v>1</v>
-      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="C4:AA4"/>
+    <mergeCell ref="C4:Y4"/>
   </mergeCells>
   <dataValidations count="18">
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showErrorMessage="1" sqref="Q7:R1048576">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showErrorMessage="1" sqref="O7:P1048576">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showErrorMessage="1" sqref="AA7:AA1048576 Y7:Y1048576">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showErrorMessage="1" sqref="Y7:Y1048576 W7:W1048576">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="N7:N1048576">
+    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="L7:L1048576">
       <formula1>validation_choices</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M7:M1048576">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K7:K1048576">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S7:T1048576 P7:P1048576 I7:K1048576 F7:G1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q7:R1048576 N7:N1048576 F7:G1048576 I7:J1048576">
       <formula1>boolean_choices</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O7">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M7">
       <formula1>ouinon</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -3593,31 +3522,31 @@
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM7 AO7">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AK7 AM7">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AD7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AB7">
       <formula1>datetype</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AC7">
+    <dataValidation type="list" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA7">
       <formula1>ouinon</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U7">
-      <formula1>$Q$7</formula1>
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S7">
+      <formula1>$O$7</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AI7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AG7">
       <formula1>validation_type</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AH7">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AF7">
       <formula1>0</formula1>
       <formula2>200</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AK7:AL7 AQ7:AS7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AI7:AJ7 AO7:AQ7">
       <formula1>ouinon</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -3627,10 +3556,10 @@
     <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="D7:D1048576">
       <formula1>attribute_groups</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W7:W1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U7:U1048576">
       <formula1>metric_types</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X7:X1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V7:V1048576">
       <formula1>metric_units</formula1>
     </dataValidation>
   </dataValidations>
@@ -3642,11 +3571,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AZ8"/>
+  <dimension ref="A1:AX8"/>
   <sheetViews>
-    <sheetView topLeftCell="T1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="V1" sqref="V1:V1048576"/>
-    </sheetView>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3659,48 +3586,46 @@
     <col min="8" max="8" width="25.140625" style="16"/>
     <col min="9" max="9" width="20"/>
     <col min="10" max="10" width="23.5703125" style="16"/>
-    <col min="11" max="11" width="23.85546875" style="16"/>
-    <col min="12" max="12" width="20.7109375" style="16"/>
-    <col min="13" max="13" width="13" style="16" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.42578125"/>
-    <col min="15" max="15" width="19.28515625"/>
-    <col min="16" max="17" width="17.28515625"/>
-    <col min="18" max="18" width="16.5703125"/>
-    <col min="19" max="19" width="19"/>
-    <col min="20" max="21" width="18.7109375"/>
+    <col min="11" max="11" width="20.7109375" style="16"/>
+    <col min="12" max="12" width="20.42578125"/>
+    <col min="13" max="13" width="19.28515625"/>
+    <col min="14" max="15" width="17.28515625"/>
+    <col min="16" max="16" width="16.5703125"/>
+    <col min="17" max="17" width="19"/>
+    <col min="18" max="19" width="18.7109375"/>
+    <col min="20" max="20" width="13.42578125"/>
+    <col min="21" max="21" width="19.85546875"/>
     <col min="22" max="22" width="13.42578125"/>
-    <col min="23" max="23" width="19.85546875"/>
-    <col min="24" max="24" width="13.42578125"/>
-    <col min="25" max="25" width="18.140625"/>
-    <col min="26" max="26" width="21"/>
-    <col min="27" max="27" width="22"/>
-    <col min="28" max="28" width="23.42578125"/>
-    <col min="29" max="29" width="14.85546875" style="16"/>
-    <col min="30" max="38" width="13.42578125"/>
-    <col min="39" max="39" width="16.85546875"/>
-    <col min="40" max="40" width="19.140625"/>
-    <col min="41" max="41" width="16.28515625"/>
-    <col min="42" max="44" width="13.42578125"/>
-    <col min="45" max="45" width="19.140625"/>
-    <col min="46" max="48" width="18.140625"/>
+    <col min="23" max="23" width="18.140625"/>
+    <col min="24" max="24" width="21"/>
+    <col min="25" max="25" width="22"/>
+    <col min="26" max="26" width="23.42578125"/>
+    <col min="27" max="27" width="14.85546875" style="16"/>
+    <col min="28" max="36" width="13.42578125"/>
+    <col min="37" max="37" width="16.85546875"/>
+    <col min="38" max="38" width="19.140625"/>
+    <col min="39" max="39" width="16.28515625"/>
+    <col min="40" max="42" width="13.42578125"/>
+    <col min="43" max="43" width="19.140625"/>
+    <col min="44" max="46" width="18.140625"/>
+    <col min="47" max="47" width="0" style="2" hidden="1"/>
+    <col min="48" max="48" width="0" style="3" hidden="1"/>
     <col min="49" max="49" width="0" style="2" hidden="1"/>
-    <col min="50" max="50" width="0" style="3" hidden="1"/>
-    <col min="51" max="51" width="0" style="2" hidden="1"/>
-    <col min="52" max="52" width="17.140625" style="2"/>
-    <col min="53" max="1023" width="17.140625"/>
+    <col min="50" max="50" width="17.140625" style="2"/>
+    <col min="51" max="1021" width="17.140625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:52" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:50" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D1" s="4"/>
       <c r="E1" s="4" t="s">
         <v>0</v>
       </c>
+      <c r="AU1"/>
+      <c r="AV1"/>
       <c r="AW1"/>
       <c r="AX1"/>
-      <c r="AY1"/>
-      <c r="AZ1"/>
-    </row>
-    <row r="2" spans="1:52" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:50" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -3713,12 +3638,12 @@
       <c r="E2" s="4" t="s">
         <v>4</v>
       </c>
+      <c r="AU2"/>
+      <c r="AV2"/>
       <c r="AW2"/>
       <c r="AX2"/>
-      <c r="AY2"/>
-      <c r="AZ2"/>
-    </row>
-    <row r="4" spans="1:52" s="19" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:50" s="19" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="25"/>
       <c r="B4" s="25"/>
       <c r="C4" s="6" t="s">
@@ -3749,13 +3674,11 @@
       <c r="X4" s="31"/>
       <c r="Y4" s="31"/>
       <c r="Z4" s="31"/>
-      <c r="AA4" s="31"/>
-      <c r="AB4" s="31"/>
-      <c r="AC4" s="7" t="s">
+      <c r="AA4" s="7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:52" s="19" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:50" s="19" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="25" t="s">
         <v>8</v>
       </c>
@@ -3775,76 +3698,70 @@
         <v>12</v>
       </c>
       <c r="G5" s="26" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="H5" s="26" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="I5" s="26" t="s">
         <v>13</v>
       </c>
       <c r="J5" s="26" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="K5" s="26" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="L5" s="26" t="s">
-        <v>238</v>
+        <v>14</v>
       </c>
       <c r="M5" s="26" t="s">
-        <v>262</v>
+        <v>15</v>
       </c>
       <c r="N5" s="26" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="O5" s="26" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="P5" s="26" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="Q5" s="26" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="R5" s="26" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="S5" s="26" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="T5" s="26" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="U5" s="26" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="V5" s="26" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="W5" s="26" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="X5" s="26" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="Y5" s="26" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="Z5" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="AA5" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="AB5" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="AC5" s="30" t="s">
+      <c r="AA5" s="30" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:52" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:50" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>29</v>
       </c>
@@ -3870,7 +3787,7 @@
         <v>36</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>37</v>
+        <v>262</v>
       </c>
       <c r="J6" s="17" t="s">
         <v>38</v>
@@ -3878,17 +3795,17 @@
       <c r="K6" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="L6" s="17" t="s">
+      <c r="L6" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="M6" s="17" t="s">
-        <v>263</v>
+      <c r="M6" s="9" t="s">
+        <v>41</v>
       </c>
       <c r="N6" s="9" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="O6" s="9" t="s">
-        <v>42</v>
+        <v>261</v>
       </c>
       <c r="P6" s="9" t="s">
         <v>43</v>
@@ -3923,21 +3840,15 @@
       <c r="Z6" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="AA6" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="AB6" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="AC6" s="20"/>
+      <c r="AA6" s="20"/>
+      <c r="AU6"/>
+      <c r="AV6"/>
       <c r="AW6"/>
       <c r="AX6"/>
-      <c r="AY6"/>
-      <c r="AZ6"/>
-    </row>
-    <row r="7" spans="1:52" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
@@ -3946,9 +3857,9 @@
       <c r="I7" s="11"/>
       <c r="J7" s="18"/>
       <c r="K7" s="18"/>
-      <c r="L7" s="18"/>
-      <c r="M7" s="18"/>
+      <c r="L7" s="11"/>
       <c r="N7" s="11"/>
+      <c r="O7" s="11"/>
       <c r="P7" s="11"/>
       <c r="Q7" s="11"/>
       <c r="R7" s="11"/>
@@ -3960,11 +3871,11 @@
       <c r="X7" s="11"/>
       <c r="Y7" s="11"/>
       <c r="Z7" s="11"/>
-      <c r="AA7" s="11"/>
+      <c r="AA7" s="18">
+        <v>1</v>
+      </c>
       <c r="AB7" s="11"/>
-      <c r="AC7" s="18">
-        <v>1</v>
-      </c>
+      <c r="AC7" s="11"/>
       <c r="AD7" s="11"/>
       <c r="AE7" s="11"/>
       <c r="AF7" s="11"/>
@@ -3982,58 +3893,56 @@
       <c r="AR7" s="11"/>
       <c r="AS7" s="11"/>
       <c r="AT7" s="11"/>
-      <c r="AU7" s="11"/>
-      <c r="AV7" s="11"/>
-      <c r="AW7" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="AY7" s="2">
+      <c r="AU7" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AW7" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>
-      <c r="AC8" s="16">
+      <c r="AA8" s="16">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D4:AB4"/>
+    <mergeCell ref="D4:Z4"/>
   </mergeCells>
   <dataValidations count="19">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM7:AN7 AS7:AU7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AK7:AL7 AQ7:AS7">
       <formula1>ouinon</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AJ7">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AH7">
       <formula1>0</formula1>
       <formula2>200</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AK7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AI7">
       <formula1>validation_type</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V7">
-      <formula1>$R$7</formula1>
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T7">
+      <formula1>$P$7</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AE7">
+    <dataValidation type="list" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AC7">
       <formula1>ouinon</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AF7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AD7">
       <formula1>datetype</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AO7 AQ7">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM7 AO7">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -4041,39 +3950,39 @@
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P7">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N7">
       <formula1>ouinon</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T7:U1048576 Q7:Q1048576 B7:B1048576 J7:L1048576 G7:H1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R7:S1048576 O7:O1048576 B7:B1048576 G7:H1048576 J7:K1048576">
       <formula1>boolean_choices</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N7:N1048576">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L7:L1048576">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="O7:O1048576">
+    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="M7:M1048576">
       <formula1>validation_choices</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showErrorMessage="1" sqref="AB7:AB1048576 Z7:Z1048576">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showErrorMessage="1" sqref="Z7:Z1048576 X7:X1048576">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="AC7:AC1048576">
+    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="AA7:AA1048576">
       <formula1>boolean_choices</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showErrorMessage="1" sqref="R7:S1048576">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showErrorMessage="1" sqref="P7:Q1048576">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="D1:D1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V1:V1048576">
+      <formula1>metric_types</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W1:W1048576">
+      <formula1>metric_units</formula1>
+    </dataValidation>
+    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="D3:D1048576 D1:D2">
       <formula1>attribute_types</formula1>
     </dataValidation>
-    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="E1:E1048576">
+    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="E3:E1048576 E1:E2">
       <formula1>attribute_groups</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X1:X1048576">
-      <formula1>metric_types</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y1:Y1048576">
-      <formula1>metric_units</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -4086,8 +3995,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4100,7 +4009,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="32" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B1" s="32"/>
       <c r="C1" s="13" t="s">
@@ -4109,10 +4018,10 @@
     </row>
     <row r="2" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C2" s="14" t="s">
         <v>0</v>
@@ -4131,13 +4040,13 @@
     </row>
     <row r="4" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B4" s="11">
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -4150,72 +4059,58 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24.7109375" style="12"/>
     <col min="2" max="2" width="19.7109375"/>
-    <col min="3" max="3" width="17.140625" style="11"/>
-    <col min="4" max="1025" width="17.140625"/>
+    <col min="3" max="1024" width="17.140625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="32" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="13" t="s">
+      <c r="C1" s="13" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="D2" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" s="14" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="D3" s="14" t="s">
+      <c r="C3" s="14" t="s">
         <v>31</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A1:B1"/>
   </mergeCells>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C1048576">
-      <formula1>boolean_choices</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
   <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -4224,7 +4119,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4239,7 +4134,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="32" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B1" s="32"/>
       <c r="C1" s="32"/>
@@ -4248,19 +4143,19 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="E2" s="9" t="s">
         <v>74</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
@@ -4268,16 +4163,16 @@
         <v>29</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C3" s="9" t="s">
         <v>37</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4291,7 +4186,7 @@
         <v>0</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="E4" s="11" t="s">
         <v>2</v>
@@ -4319,7 +4214,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4331,7 +4226,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="32" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B1" s="32"/>
       <c r="C1" s="13" t="s">
@@ -4340,10 +4235,10 @@
     </row>
     <row r="2" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C2" s="14" t="s">
         <v>0</v>
@@ -4354,7 +4249,7 @@
         <v>29</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C3" s="14" t="s">
         <v>31</v>
@@ -4365,7 +4260,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -4389,7 +4284,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4400,7 +4295,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="32" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="B1" s="32"/>
     </row>
@@ -4409,7 +4304,7 @@
         <v>29</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
     </row>
     <row r="3" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
@@ -4417,12 +4312,12 @@
         <v>29</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -4430,7 +4325,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -4464,7 +4359,7 @@
   <sheetData>
     <row r="1" spans="1:2" s="28" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>5</v>
@@ -4472,7 +4367,7 @@
     </row>
     <row r="2" spans="1:2" s="28" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="26" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="B2" s="13" t="s">
         <v>0</v>
@@ -4488,34 +4383,34 @@
     </row>
     <row r="4" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="B4" s="27" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="B5" s="28" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="B6" s="28" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="B7" s="28" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Corrected validation errors and removed junk characters
</commit_message>
<xml_diff>
--- a/Resources/fixtures/minimal/init.xlsx
+++ b/Resources/fixtures/minimal/init.xlsx
@@ -197,7 +197,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="262">
   <si>
     <t>en_US</t>
   </si>
@@ -371,9 +371,6 @@
   </si>
   <si>
     <t>global</t>
-  </si>
-  <si>
-    <t>1 - tous</t>
   </si>
   <si>
     <t>name</t>
@@ -1954,32 +1951,32 @@
   <sheetData>
     <row r="1" spans="1:2" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A1" s="22" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="21" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B5" s="23" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B6" s="24" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B7" s="24" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B8" s="24" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -1987,7 +1984,7 @@
     </row>
     <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="21" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -1995,127 +1992,127 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B12" s="23" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B15" s="21" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="22" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B22" s="21" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="26" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B26" s="21" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="29" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="31" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B31" s="21" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B34" s="24" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="36" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B36" s="21" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="38" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="39" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="41" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B41" s="21" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="43" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="45" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B45" s="21" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="47" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A50" s="29" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B52" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
   </sheetData>
@@ -2139,10 +2136,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -2150,18 +2147,18 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
   </sheetData>
@@ -2186,10 +2183,10 @@
   <sheetData>
     <row r="1" spans="1:2" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>102</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -2197,12 +2194,12 @@
         <v>29</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B3" t="s">
         <v>56</v>
@@ -2210,90 +2207,90 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B5" t="s">
         <v>106</v>
-      </c>
-      <c r="B5" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>107</v>
+      </c>
+      <c r="B6" t="s">
         <v>108</v>
-      </c>
-      <c r="B6" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>109</v>
+      </c>
+      <c r="B7" t="s">
         <v>110</v>
-      </c>
-      <c r="B7" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>111</v>
+      </c>
+      <c r="B8" t="s">
         <v>112</v>
-      </c>
-      <c r="B8" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>113</v>
+      </c>
+      <c r="B9" t="s">
         <v>114</v>
-      </c>
-      <c r="B9" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>115</v>
+      </c>
+      <c r="B10" t="s">
         <v>116</v>
-      </c>
-      <c r="B10" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>117</v>
+      </c>
+      <c r="B11" t="s">
         <v>118</v>
-      </c>
-      <c r="B11" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>119</v>
+      </c>
+      <c r="B12" t="s">
         <v>120</v>
-      </c>
-      <c r="B12" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>121</v>
+      </c>
+      <c r="B13" t="s">
         <v>122</v>
-      </c>
-      <c r="B13" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>123</v>
+      </c>
+      <c r="B14" t="s">
         <v>124</v>
-      </c>
-      <c r="B14" t="s">
-        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -2323,10 +2320,10 @@
   <sheetData>
     <row r="1" spans="1:2" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>102</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -2334,79 +2331,79 @@
         <v>29</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -2436,7 +2433,7 @@
   <sheetData>
     <row r="1" spans="1:1024" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B1" s="9"/>
       <c r="AMJ1"/>
@@ -2446,704 +2443,704 @@
         <v>32</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AMJ2"/>
     </row>
     <row r="3" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="6" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="7" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="8" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="9" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="10" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="11" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B11" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="12" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="13" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B13" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="14" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B14" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="15" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B15" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="16" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B16" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B17" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B18" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B19" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B20" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B21" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B22" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B23" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B24" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B25" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B26" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B27" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B28" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B29" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B30" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B31" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B32" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B33" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B34" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B35" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B36" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B37" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B38" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B39" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B40" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B41" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B42" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B43" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B44" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B45" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B46" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B47" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B48" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B49" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B50" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B51" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B52" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B53" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B54" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B55" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B56" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B57" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B58" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B59" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B60" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B61" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B62" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B63" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B64" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B65" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B66" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B67" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B68" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B69" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B70" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B71" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B72" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B73" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B74" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B75" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B76" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B77" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B78" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B79" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B80" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B81" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B82" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B84" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B85" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B86" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B87" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B88" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B89" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
   </sheetData>
@@ -3195,7 +3192,7 @@
   <sheetData>
     <row r="1" spans="1:48" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="24" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
@@ -3261,19 +3258,19 @@
         <v>12</v>
       </c>
       <c r="F5" s="26" t="s">
+        <v>229</v>
+      </c>
+      <c r="G5" s="26" t="s">
         <v>230</v>
-      </c>
-      <c r="G5" s="26" t="s">
-        <v>231</v>
       </c>
       <c r="H5" s="26" t="s">
         <v>13</v>
       </c>
       <c r="I5" s="26" t="s">
+        <v>231</v>
+      </c>
+      <c r="J5" s="26" t="s">
         <v>232</v>
-      </c>
-      <c r="J5" s="26" t="s">
-        <v>233</v>
       </c>
       <c r="K5" s="26" t="s">
         <v>14</v>
@@ -3344,7 +3341,7 @@
         <v>36</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="I6" s="17" t="s">
         <v>38</v>
@@ -3362,7 +3359,7 @@
         <v>42</v>
       </c>
       <c r="N6" s="9" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="O6" s="9" t="s">
         <v>43</v>
@@ -3467,13 +3464,13 @@
     </row>
     <row r="8" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" t="s">
         <v>59</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" s="10" t="s">
         <v>60</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>61</v>
       </c>
       <c r="D8" s="10" t="s">
         <v>57</v>
@@ -3498,7 +3495,7 @@
   <mergeCells count="1">
     <mergeCell ref="C4:Y4"/>
   </mergeCells>
-  <dataValidations count="18">
+  <dataValidations count="12">
     <dataValidation type="whole" operator="greaterThan" allowBlank="1" showErrorMessage="1" sqref="O7:P1048576">
       <formula1>0</formula1>
     </dataValidation>
@@ -3522,32 +3519,8 @@
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AK7 AM7">
-      <formula1>0</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AB7">
-      <formula1>datetype</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation type="list" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA7">
-      <formula1>ouinon</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
     <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S7">
       <formula1>$O$7</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AG7">
-      <formula1>validation_type</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AF7">
-      <formula1>0</formula1>
-      <formula2>200</formula2>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AI7:AJ7 AO7:AQ7">
-      <formula1>ouinon</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="C7:C1048576">
@@ -3608,9 +3581,9 @@
     <col min="40" max="42" width="13.42578125"/>
     <col min="43" max="43" width="19.140625"/>
     <col min="44" max="46" width="18.140625"/>
-    <col min="47" max="47" width="0" style="2" hidden="1"/>
-    <col min="48" max="48" width="0" style="3" hidden="1"/>
-    <col min="49" max="49" width="0" style="2" hidden="1"/>
+    <col min="47" max="47" width="9.140625" style="2"/>
+    <col min="48" max="48" width="9.140625" style="3"/>
+    <col min="49" max="49" width="9.140625" style="2"/>
     <col min="50" max="50" width="17.140625" style="2"/>
     <col min="51" max="1021" width="17.140625"/>
   </cols>
@@ -3698,19 +3671,19 @@
         <v>12</v>
       </c>
       <c r="G5" s="26" t="s">
+        <v>229</v>
+      </c>
+      <c r="H5" s="26" t="s">
         <v>230</v>
-      </c>
-      <c r="H5" s="26" t="s">
-        <v>231</v>
       </c>
       <c r="I5" s="26" t="s">
         <v>13</v>
       </c>
       <c r="J5" s="26" t="s">
+        <v>231</v>
+      </c>
+      <c r="K5" s="26" t="s">
         <v>232</v>
-      </c>
-      <c r="K5" s="26" t="s">
-        <v>233</v>
       </c>
       <c r="L5" s="26" t="s">
         <v>14</v>
@@ -3787,7 +3760,7 @@
         <v>36</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="J6" s="17" t="s">
         <v>38</v>
@@ -3805,7 +3778,7 @@
         <v>42</v>
       </c>
       <c r="O6" s="9" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="P6" s="9" t="s">
         <v>43</v>
@@ -3893,16 +3866,10 @@
       <c r="AR7" s="11"/>
       <c r="AS7" s="11"/>
       <c r="AT7" s="11"/>
-      <c r="AU7" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="AW7" s="2">
-        <v>1</v>
-      </c>
     </row>
     <row r="8" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -3917,33 +3884,9 @@
   <mergeCells count="1">
     <mergeCell ref="D4:Z4"/>
   </mergeCells>
-  <dataValidations count="19">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AK7:AL7 AQ7:AS7">
-      <formula1>ouinon</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AH7">
-      <formula1>0</formula1>
-      <formula2>200</formula2>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AI7">
-      <formula1>validation_type</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
+  <dataValidations count="13">
     <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T7">
       <formula1>$P$7</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation type="list" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AC7">
-      <formula1>ouinon</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AD7">
-      <formula1>datetype</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM7 AO7">
-      <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showErrorMessage="1" sqref="F7">
@@ -3972,16 +3915,16 @@
     <dataValidation type="whole" operator="greaterThan" allowBlank="1" showErrorMessage="1" sqref="P7:Q1048576">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V1:V1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V4:V1048576">
       <formula1>metric_types</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W1:W1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W4:W1048576">
       <formula1>metric_units</formula1>
     </dataValidation>
-    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="D3:D1048576 D1:D2">
+    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="D4:D1048576">
       <formula1>attribute_types</formula1>
     </dataValidation>
-    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="E3:E1048576 E1:E2">
+    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="E4:E1048576">
       <formula1>attribute_groups</formula1>
     </dataValidation>
   </dataValidations>
@@ -4009,7 +3952,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="32" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B1" s="32"/>
       <c r="C1" s="13" t="s">
@@ -4018,10 +3961,10 @@
     </row>
     <row r="2" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" s="9" t="s">
         <v>63</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>64</v>
       </c>
       <c r="C2" s="14" t="s">
         <v>0</v>
@@ -4046,7 +3989,7 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -4075,7 +4018,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="32" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B1" s="32"/>
       <c r="C1" s="13" t="s">
@@ -4087,7 +4030,7 @@
         <v>8</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C2" s="14" t="s">
         <v>0</v>
@@ -4095,7 +4038,7 @@
     </row>
     <row r="3" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>29</v>
@@ -4134,7 +4077,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="32" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B1" s="32"/>
       <c r="C1" s="32"/>
@@ -4143,19 +4086,19 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="C2" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="D2" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="E2" s="9" t="s">
         <v>73</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
@@ -4163,16 +4106,16 @@
         <v>29</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C3" s="9" t="s">
         <v>37</v>
       </c>
       <c r="D3" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="E3" s="9" t="s">
         <v>85</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4186,7 +4129,7 @@
         <v>0</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E4" s="11" t="s">
         <v>2</v>
@@ -4226,7 +4169,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="32" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B1" s="32"/>
       <c r="C1" s="13" t="s">
@@ -4235,10 +4178,10 @@
     </row>
     <row r="2" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" s="9" t="s">
         <v>98</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>99</v>
       </c>
       <c r="C2" s="14" t="s">
         <v>0</v>
@@ -4249,7 +4192,7 @@
         <v>29</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C3" s="14" t="s">
         <v>31</v>
@@ -4260,7 +4203,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -4295,7 +4238,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="32" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B1" s="32"/>
     </row>
@@ -4304,7 +4247,7 @@
         <v>29</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="3" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
@@ -4312,12 +4255,12 @@
         <v>29</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -4325,7 +4268,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -4359,7 +4302,7 @@
   <sheetData>
     <row r="1" spans="1:2" s="28" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>5</v>
@@ -4367,7 +4310,7 @@
     </row>
     <row r="2" spans="1:2" s="28" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="26" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B2" s="13" t="s">
         <v>0</v>
@@ -4383,34 +4326,34 @@
     </row>
     <row r="4" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
+        <v>237</v>
+      </c>
+      <c r="B4" s="27" t="s">
         <v>238</v>
-      </c>
-      <c r="B4" s="27" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
+        <v>239</v>
+      </c>
+      <c r="B5" s="28" t="s">
         <v>240</v>
-      </c>
-      <c r="B5" s="28" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
+        <v>241</v>
+      </c>
+      <c r="B6" s="28" t="s">
         <v>242</v>
-      </c>
-      <c r="B6" s="28" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
+        <v>243</v>
+      </c>
+      <c r="B7" s="28" t="s">
         <v>244</v>
-      </c>
-      <c r="B7" s="28" t="s">
-        <v>245</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added 'OTHER' attribute group
</commit_message>
<xml_diff>
--- a/Resources/fixtures/minimal/init.xlsx
+++ b/Resources/fixtures/minimal/init.xlsx
@@ -197,7 +197,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="264">
   <si>
     <t>en_US</t>
   </si>
@@ -1094,6 +1094,12 @@
   </si>
   <si>
     <t>available_locales</t>
+  </si>
+  <si>
+    <t>OTHER</t>
+  </si>
+  <si>
+    <t>Other</t>
   </si>
 </sst>
 </file>
@@ -3936,7 +3942,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection sqref="A1:B1"/>
@@ -3990,6 +3996,17 @@
       </c>
       <c r="C4" t="s">
         <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="12" t="s">
+        <v>262</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>263</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated doc and init.xslx file to add new Metric types
</commit_message>
<xml_diff>
--- a/Resources/fixtures/minimal/init.xlsx
+++ b/Resources/fixtures/minimal/init.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="6570" tabRatio="226"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="6570" tabRatio="533" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="10" r:id="rId1"/>
@@ -197,7 +197,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="267">
   <si>
     <t>en_US</t>
   </si>
@@ -1100,6 +1100,15 @@
   </si>
   <si>
     <t>Other</t>
+  </si>
+  <si>
+    <t>Voltage</t>
+  </si>
+  <si>
+    <t>Intensity</t>
+  </si>
+  <si>
+    <t>Resistance</t>
   </si>
 </sst>
 </file>
@@ -1948,7 +1957,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2311,10 +2320,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="B14" sqref="A12:B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2410,6 +2419,30 @@
       </c>
       <c r="B11" t="s">
         <v>82</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>264</v>
+      </c>
+      <c r="B12" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>265</v>
+      </c>
+      <c r="B13" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>266</v>
+      </c>
+      <c r="B14" t="s">
+        <v>266</v>
       </c>
     </row>
   </sheetData>
@@ -4309,7 +4342,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>